<commit_message>
Add button click methods [[ERROR]]
</commit_message>
<xml_diff>
--- a/_DESIGN/Book4.xlsx
+++ b/_DESIGN/Book4.xlsx
@@ -9,11 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8010"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8010" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="83">
   <si>
     <t>button11</t>
   </si>
@@ -268,6 +269,12 @@
   </si>
   <si>
     <t>button99</t>
+  </si>
+  <si>
+    <t>game</t>
+  </si>
+  <si>
+    <t>position</t>
   </si>
 </sst>
 </file>
@@ -283,7 +290,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -308,6 +315,30 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF0070C0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -321,12 +352,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -643,8 +681,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K21" sqref="K21"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I9" sqref="A1:I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1240,344 +1278,344 @@
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="K11" s="1" t="str">
-        <f>"&lt;Button android:id="&amp;CHAR(34)&amp;"@+id/button11"&amp;CHAR(34)&amp;" android:layout_width="&amp;CHAR(34)&amp;"wrap_content"&amp;CHAR(34)&amp;" android:layout_height="&amp;CHAR(34)&amp;"wrap_content"&amp;CHAR(34)&amp;" android:layout_marginLeft="&amp;CHAR(34)&amp;"8dp"&amp;CHAR(34)&amp;" android:layout_marginStart="&amp;CHAR(34)&amp;"8dp"&amp;CHAR(34)&amp;" android:layout_marginTop="&amp;CHAR(34)&amp;"16dp"&amp;CHAR(34)&amp;" android:minWidth="&amp;CHAR(34)&amp;"40dp"&amp;CHAR(34)&amp;" android:text="&amp;CHAR(34)&amp;"O"&amp;CHAR(34)&amp;" app:layout_constraintEnd_toStartOf="&amp;CHAR(34)&amp;"@id/button12"&amp;CHAR(34)&amp;" app:layout_constraintHorizontal_weight="&amp;CHAR(34)&amp;"1"&amp;CHAR(34)&amp;" app:layout_constraintStart_toStartOf="&amp;CHAR(34)&amp;"parent"&amp;CHAR(34)&amp;" app:layout_constraintTop_toBottomOf="&amp;CHAR(34)&amp;"@id/imageView"&amp;CHAR(34)&amp;" /&gt;"</f>
-        <v>&lt;Button android:id="@+id/button11" android:layout_width="wrap_content" android:layout_height="wrap_content" android:layout_marginLeft="8dp" android:layout_marginStart="8dp" android:layout_marginTop="16dp" android:minWidth="40dp" android:text="O" app:layout_constraintEnd_toStartOf="@id/button12" app:layout_constraintHorizontal_weight="1" app:layout_constraintStart_toStartOf="parent" app:layout_constraintTop_toBottomOf="@id/imageView" /&gt;</v>
-      </c>
-      <c r="L11" s="4" t="str">
-        <f>"&lt;Button android:id="&amp;CHAR(34)&amp;"@+id/"&amp;L1&amp;CHAR(34)&amp;" android:layout_width="&amp;CHAR(34)&amp;"wrap_content"&amp;CHAR(34)&amp;" android:layout_height="&amp;CHAR(34)&amp;"wrap_content"&amp;CHAR(34)&amp;" android:layout_marginTop="&amp;CHAR(34)&amp;"16dp"&amp;CHAR(34)&amp;" android:minWidth="&amp;CHAR(34)&amp;"40dp"&amp;CHAR(34)&amp;" android:text="&amp;CHAR(34)&amp;"O"&amp;CHAR(34)&amp;" app:layout_constraintEnd_toStartOf="&amp;CHAR(34)&amp;"@id/"&amp;M1&amp;CHAR(34)&amp;" app:layout_constraintHorizontal_weight="&amp;CHAR(34)&amp;"1"&amp;CHAR(34)&amp;" app:layout_constraintStart_toEndOf="&amp;CHAR(34)&amp;"@+id/"&amp;K1&amp;CHAR(34)&amp;" app:layout_constraintTop_toBottomOf="&amp;CHAR(34)&amp;"@id/imageView"&amp;CHAR(34)&amp;" /&gt;"</f>
-        <v>&lt;Button android:id="@+id/button12" android:layout_width="wrap_content" android:layout_height="wrap_content" android:layout_marginTop="16dp" android:minWidth="40dp" android:text="O" app:layout_constraintEnd_toStartOf="@id/button13" app:layout_constraintHorizontal_weight="1" app:layout_constraintStart_toEndOf="@+id/button11" app:layout_constraintTop_toBottomOf="@id/imageView" /&gt;</v>
-      </c>
-      <c r="M11" s="4" t="str">
-        <f t="shared" ref="M11:R11" si="10">"&lt;Button android:id="&amp;CHAR(34)&amp;"@+id/"&amp;M1&amp;CHAR(34)&amp;" android:layout_width="&amp;CHAR(34)&amp;"wrap_content"&amp;CHAR(34)&amp;" android:layout_height="&amp;CHAR(34)&amp;"wrap_content"&amp;CHAR(34)&amp;" android:layout_marginTop="&amp;CHAR(34)&amp;"16dp"&amp;CHAR(34)&amp;" android:minWidth="&amp;CHAR(34)&amp;"40dp"&amp;CHAR(34)&amp;" android:text="&amp;CHAR(34)&amp;"O"&amp;CHAR(34)&amp;" app:layout_constraintEnd_toStartOf="&amp;CHAR(34)&amp;"@id/"&amp;N1&amp;CHAR(34)&amp;" app:layout_constraintHorizontal_weight="&amp;CHAR(34)&amp;"1"&amp;CHAR(34)&amp;" app:layout_constraintStart_toEndOf="&amp;CHAR(34)&amp;"@+id/"&amp;L1&amp;CHAR(34)&amp;" app:layout_constraintTop_toBottomOf="&amp;CHAR(34)&amp;"@id/imageView"&amp;CHAR(34)&amp;" /&gt;"</f>
-        <v>&lt;Button android:id="@+id/button13" android:layout_width="wrap_content" android:layout_height="wrap_content" android:layout_marginTop="16dp" android:minWidth="40dp" android:text="O" app:layout_constraintEnd_toStartOf="@id/button14" app:layout_constraintHorizontal_weight="1" app:layout_constraintStart_toEndOf="@+id/button12" app:layout_constraintTop_toBottomOf="@id/imageView" /&gt;</v>
-      </c>
-      <c r="N11" s="4" t="str">
+        <f>"&lt;Button android:id="&amp;CHAR(34)&amp;"@+id/"&amp;K1&amp;CHAR(34)&amp;" android:layout_width="&amp;CHAR(34)&amp;"wrap_content"&amp;CHAR(34)&amp;" android:layout_height="&amp;CHAR(34)&amp;"wrap_content"&amp;CHAR(34)&amp;" android:layout_marginLeft="&amp;CHAR(34)&amp;"8dp"&amp;CHAR(34)&amp;" android:layout_marginStart="&amp;CHAR(34)&amp;"8dp"&amp;CHAR(34)&amp;" android:minWidth="&amp;CHAR(34)&amp;"40dp"&amp;CHAR(34)&amp;" android:onClick="&amp;CHAR(34)&amp;K1&amp;CHAR(34)&amp;" app:layout_constraintEnd_toStartOf="&amp;CHAR(34)&amp;"@id/button12"&amp;CHAR(34)&amp;" app:layout_constraintHorizontal_weight="&amp;CHAR(34)&amp;"1"&amp;CHAR(34)&amp;" app:layout_constraintStart_toStartOf="&amp;CHAR(34)&amp;"parent"&amp;CHAR(34)&amp;" app:layout_constraintTop_toBottomOf="&amp;CHAR(34)&amp;"@id/imageView"&amp;CHAR(34)&amp;" /&gt;"</f>
+        <v>&lt;Button android:id="@+id/button11" android:layout_width="wrap_content" android:layout_height="wrap_content" android:layout_marginLeft="8dp" android:layout_marginStart="8dp" android:minWidth="40dp" android:onClick="button11" app:layout_constraintEnd_toStartOf="@id/button12" app:layout_constraintHorizontal_weight="1" app:layout_constraintStart_toStartOf="parent" app:layout_constraintTop_toBottomOf="@id/imageView" /&gt;</v>
+      </c>
+      <c r="L11" s="5" t="str">
+        <f>"&lt;Button android:id="&amp;CHAR(34)&amp;"@+id/"&amp;L1&amp;CHAR(34)&amp;" android:layout_width="&amp;CHAR(34)&amp;"wrap_content"&amp;CHAR(34)&amp;" android:layout_height="&amp;CHAR(34)&amp;"wrap_content"&amp;CHAR(34)&amp;" android:minWidth="&amp;CHAR(34)&amp;"40dp"&amp;CHAR(34)&amp;" android:onClick="&amp;CHAR(34)&amp;L1&amp;CHAR(34)&amp;" app:layout_constraintEnd_toStartOf="&amp;CHAR(34)&amp;"@id/"&amp;M1&amp;CHAR(34)&amp;" app:layout_constraintHorizontal_weight="&amp;CHAR(34)&amp;"1"&amp;CHAR(34)&amp;" app:layout_constraintStart_toEndOf="&amp;CHAR(34)&amp;"@+id/"&amp;K1&amp;CHAR(34)&amp;" app:layout_constraintTop_toBottomOf="&amp;CHAR(34)&amp;"@id/imageView"&amp;CHAR(34)&amp;" /&gt;"</f>
+        <v>&lt;Button android:id="@+id/button12" android:layout_width="wrap_content" android:layout_height="wrap_content" android:minWidth="40dp" android:onClick="button12" app:layout_constraintEnd_toStartOf="@id/button13" app:layout_constraintHorizontal_weight="1" app:layout_constraintStart_toEndOf="@+id/button11" app:layout_constraintTop_toBottomOf="@id/imageView" /&gt;</v>
+      </c>
+      <c r="M11" s="5" t="str">
+        <f t="shared" ref="M11:R11" si="10">"&lt;Button android:id="&amp;CHAR(34)&amp;"@+id/"&amp;M1&amp;CHAR(34)&amp;" android:layout_width="&amp;CHAR(34)&amp;"wrap_content"&amp;CHAR(34)&amp;" android:layout_height="&amp;CHAR(34)&amp;"wrap_content"&amp;CHAR(34)&amp;" android:minWidth="&amp;CHAR(34)&amp;"40dp"&amp;CHAR(34)&amp;" android:onClick="&amp;CHAR(34)&amp;M1&amp;CHAR(34)&amp;" app:layout_constraintEnd_toStartOf="&amp;CHAR(34)&amp;"@id/"&amp;N1&amp;CHAR(34)&amp;" app:layout_constraintHorizontal_weight="&amp;CHAR(34)&amp;"1"&amp;CHAR(34)&amp;" app:layout_constraintStart_toEndOf="&amp;CHAR(34)&amp;"@+id/"&amp;L1&amp;CHAR(34)&amp;" app:layout_constraintTop_toBottomOf="&amp;CHAR(34)&amp;"@id/imageView"&amp;CHAR(34)&amp;" /&gt;"</f>
+        <v>&lt;Button android:id="@+id/button13" android:layout_width="wrap_content" android:layout_height="wrap_content" android:minWidth="40dp" android:onClick="button13" app:layout_constraintEnd_toStartOf="@id/button14" app:layout_constraintHorizontal_weight="1" app:layout_constraintStart_toEndOf="@+id/button12" app:layout_constraintTop_toBottomOf="@id/imageView" /&gt;</v>
+      </c>
+      <c r="N11" s="5" t="str">
         <f t="shared" si="10"/>
-        <v>&lt;Button android:id="@+id/button14" android:layout_width="wrap_content" android:layout_height="wrap_content" android:layout_marginTop="16dp" android:minWidth="40dp" android:text="O" app:layout_constraintEnd_toStartOf="@id/button15" app:layout_constraintHorizontal_weight="1" app:layout_constraintStart_toEndOf="@+id/button13" app:layout_constraintTop_toBottomOf="@id/imageView" /&gt;</v>
-      </c>
-      <c r="O11" s="4" t="str">
+        <v>&lt;Button android:id="@+id/button14" android:layout_width="wrap_content" android:layout_height="wrap_content" android:minWidth="40dp" android:onClick="button14" app:layout_constraintEnd_toStartOf="@id/button15" app:layout_constraintHorizontal_weight="1" app:layout_constraintStart_toEndOf="@+id/button13" app:layout_constraintTop_toBottomOf="@id/imageView" /&gt;</v>
+      </c>
+      <c r="O11" s="5" t="str">
         <f t="shared" si="10"/>
-        <v>&lt;Button android:id="@+id/button15" android:layout_width="wrap_content" android:layout_height="wrap_content" android:layout_marginTop="16dp" android:minWidth="40dp" android:text="O" app:layout_constraintEnd_toStartOf="@id/button16" app:layout_constraintHorizontal_weight="1" app:layout_constraintStart_toEndOf="@+id/button14" app:layout_constraintTop_toBottomOf="@id/imageView" /&gt;</v>
-      </c>
-      <c r="P11" s="4" t="str">
+        <v>&lt;Button android:id="@+id/button15" android:layout_width="wrap_content" android:layout_height="wrap_content" android:minWidth="40dp" android:onClick="button15" app:layout_constraintEnd_toStartOf="@id/button16" app:layout_constraintHorizontal_weight="1" app:layout_constraintStart_toEndOf="@+id/button14" app:layout_constraintTop_toBottomOf="@id/imageView" /&gt;</v>
+      </c>
+      <c r="P11" s="5" t="str">
         <f t="shared" si="10"/>
-        <v>&lt;Button android:id="@+id/button16" android:layout_width="wrap_content" android:layout_height="wrap_content" android:layout_marginTop="16dp" android:minWidth="40dp" android:text="O" app:layout_constraintEnd_toStartOf="@id/button17" app:layout_constraintHorizontal_weight="1" app:layout_constraintStart_toEndOf="@+id/button15" app:layout_constraintTop_toBottomOf="@id/imageView" /&gt;</v>
-      </c>
-      <c r="Q11" s="4" t="str">
+        <v>&lt;Button android:id="@+id/button16" android:layout_width="wrap_content" android:layout_height="wrap_content" android:minWidth="40dp" android:onClick="button16" app:layout_constraintEnd_toStartOf="@id/button17" app:layout_constraintHorizontal_weight="1" app:layout_constraintStart_toEndOf="@+id/button15" app:layout_constraintTop_toBottomOf="@id/imageView" /&gt;</v>
+      </c>
+      <c r="Q11" s="5" t="str">
         <f t="shared" si="10"/>
-        <v>&lt;Button android:id="@+id/button17" android:layout_width="wrap_content" android:layout_height="wrap_content" android:layout_marginTop="16dp" android:minWidth="40dp" android:text="O" app:layout_constraintEnd_toStartOf="@id/button18" app:layout_constraintHorizontal_weight="1" app:layout_constraintStart_toEndOf="@+id/button16" app:layout_constraintTop_toBottomOf="@id/imageView" /&gt;</v>
-      </c>
-      <c r="R11" s="4" t="str">
+        <v>&lt;Button android:id="@+id/button17" android:layout_width="wrap_content" android:layout_height="wrap_content" android:minWidth="40dp" android:onClick="button17" app:layout_constraintEnd_toStartOf="@id/button18" app:layout_constraintHorizontal_weight="1" app:layout_constraintStart_toEndOf="@+id/button16" app:layout_constraintTop_toBottomOf="@id/imageView" /&gt;</v>
+      </c>
+      <c r="R11" s="5" t="str">
         <f t="shared" si="10"/>
-        <v>&lt;Button android:id="@+id/button18" android:layout_width="wrap_content" android:layout_height="wrap_content" android:layout_marginTop="16dp" android:minWidth="40dp" android:text="O" app:layout_constraintEnd_toStartOf="@id/button19" app:layout_constraintHorizontal_weight="1" app:layout_constraintStart_toEndOf="@+id/button17" app:layout_constraintTop_toBottomOf="@id/imageView" /&gt;</v>
-      </c>
-      <c r="S11" s="1" t="str">
-        <f>"&lt;Button android:id="&amp;CHAR(34)&amp;"@+id/"&amp;S1&amp;CHAR(34)&amp;" android:layout_width="&amp;CHAR(34)&amp;"wrap_content"&amp;CHAR(34)&amp;" android:layout_height="&amp;CHAR(34)&amp;"wrap_content"&amp;CHAR(34)&amp;" android:layout_marginEnd="&amp;CHAR(34)&amp;"8dp"&amp;CHAR(34)&amp;" android:layout_marginRight="&amp;CHAR(34)&amp;"8dp"&amp;CHAR(34)&amp;" android:layout_marginTop="&amp;CHAR(34)&amp;"16dp"&amp;CHAR(34)&amp;" android:minWidth="&amp;CHAR(34)&amp;"40dp"&amp;CHAR(34)&amp;" android:text="&amp;CHAR(34)&amp;"O"&amp;CHAR(34)&amp;" app:layout_constraintEnd_toEndOf="&amp;CHAR(34)&amp;"parent"&amp;CHAR(34)&amp;" app:layout_constraintHorizontal_weight="&amp;CHAR(34)&amp;"1"&amp;CHAR(34)&amp;" app:layout_constraintStart_toEndOf="&amp;CHAR(34)&amp;"@id/"&amp;R1&amp;CHAR(34)&amp;" app:layout_constraintTop_toBottomOf="&amp;CHAR(34)&amp;"@id/imageView"&amp;CHAR(34)&amp;" /&gt;"</f>
-        <v>&lt;Button android:id="@+id/button19" android:layout_width="wrap_content" android:layout_height="wrap_content" android:layout_marginEnd="8dp" android:layout_marginRight="8dp" android:layout_marginTop="16dp" android:minWidth="40dp" android:text="O" app:layout_constraintEnd_toEndOf="parent" app:layout_constraintHorizontal_weight="1" app:layout_constraintStart_toEndOf="@id/button18" app:layout_constraintTop_toBottomOf="@id/imageView" /&gt;</v>
+        <v>&lt;Button android:id="@+id/button18" android:layout_width="wrap_content" android:layout_height="wrap_content" android:minWidth="40dp" android:onClick="button18" app:layout_constraintEnd_toStartOf="@id/button19" app:layout_constraintHorizontal_weight="1" app:layout_constraintStart_toEndOf="@+id/button17" app:layout_constraintTop_toBottomOf="@id/imageView" /&gt;</v>
+      </c>
+      <c r="S11" s="7" t="str">
+        <f>"&lt;Button android:id="&amp;CHAR(34)&amp;"@+id/"&amp;S1&amp;CHAR(34)&amp;" android:layout_width="&amp;CHAR(34)&amp;"wrap_content"&amp;CHAR(34)&amp;" android:layout_height="&amp;CHAR(34)&amp;"wrap_content"&amp;CHAR(34)&amp;" android:layout_marginEnd="&amp;CHAR(34)&amp;"8dp"&amp;CHAR(34)&amp;" android:layout_marginRight="&amp;CHAR(34)&amp;"8dp"&amp;CHAR(34)&amp;" android:minWidth="&amp;CHAR(34)&amp;"40dp"&amp;CHAR(34)&amp;" android:onClick="&amp;CHAR(34)&amp;S1&amp;CHAR(34)&amp;" app:layout_constraintEnd_toEndOf="&amp;CHAR(34)&amp;"parent"&amp;CHAR(34)&amp;" app:layout_constraintHorizontal_weight="&amp;CHAR(34)&amp;"1"&amp;CHAR(34)&amp;" app:layout_constraintStart_toEndOf="&amp;CHAR(34)&amp;"@id/"&amp;R1&amp;CHAR(34)&amp;" app:layout_constraintTop_toBottomOf="&amp;CHAR(34)&amp;"@id/imageView"&amp;CHAR(34)&amp;" /&gt;"</f>
+        <v>&lt;Button android:id="@+id/button19" android:layout_width="wrap_content" android:layout_height="wrap_content" android:layout_marginEnd="8dp" android:layout_marginRight="8dp" android:minWidth="40dp" android:onClick="button19" app:layout_constraintEnd_toEndOf="parent" app:layout_constraintHorizontal_weight="1" app:layout_constraintStart_toEndOf="@id/button18" app:layout_constraintTop_toBottomOf="@id/imageView" /&gt;</v>
       </c>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="K12" s="4" t="str">
-        <f>"&lt;Button android:id="&amp;CHAR(34)&amp;"@+id/"&amp;K2&amp;CHAR(34)&amp;" android:layout_width="&amp;CHAR(34)&amp;"wrap_content"&amp;CHAR(34)&amp;" android:layout_height="&amp;CHAR(34)&amp;"wrap_content"&amp;CHAR(34)&amp;" android:layout_marginLeft="&amp;CHAR(34)&amp;"8dp"&amp;CHAR(34)&amp;" android:layout_marginStart="&amp;CHAR(34)&amp;"8dp"&amp;CHAR(34)&amp;" android:minWidth="&amp;CHAR(34)&amp;"40dp"&amp;CHAR(34)&amp;" android:text="&amp;CHAR(34)&amp;"O"&amp;CHAR(34)&amp;" app:layout_constraintEnd_toStartOf="&amp;CHAR(34)&amp;"@id/"&amp;L2&amp;CHAR(34)&amp;" app:layout_constraintHorizontal_weight="&amp;CHAR(34)&amp;"1"&amp;CHAR(34)&amp;" app:layout_constraintStart_toStartOf="&amp;CHAR(34)&amp;"parent"&amp;CHAR(34)&amp;" app:layout_constraintTop_toBottomOf="&amp;CHAR(34)&amp;"@id/"&amp;K1&amp;CHAR(34)&amp;" /&gt;"</f>
-        <v>&lt;Button android:id="@+id/button21" android:layout_width="wrap_content" android:layout_height="wrap_content" android:layout_marginLeft="8dp" android:layout_marginStart="8dp" android:minWidth="40dp" android:text="O" app:layout_constraintEnd_toStartOf="@id/button22" app:layout_constraintHorizontal_weight="1" app:layout_constraintStart_toStartOf="parent" app:layout_constraintTop_toBottomOf="@id/button11" /&gt;</v>
-      </c>
-      <c r="L12" t="str">
-        <f>"&lt;Button android:id="&amp;CHAR(34)&amp;"@+id/"&amp;L2&amp;CHAR(34)&amp;" android:layout_width="&amp;CHAR(34)&amp;"wrap_content"&amp;CHAR(34)&amp;" android:layout_height="&amp;CHAR(34)&amp;"wrap_content"&amp;CHAR(34)&amp;" android:minWidth="&amp;CHAR(34)&amp;"40dp"&amp;CHAR(34)&amp;" android:text="&amp;CHAR(34)&amp;"O"&amp;CHAR(34)&amp;" app:layout_constraintEnd_toStartOf="&amp;CHAR(34)&amp;"@id/"&amp;M2&amp;CHAR(34)&amp;" app:layout_constraintHorizontal_weight="&amp;CHAR(34)&amp;"1"&amp;CHAR(34)&amp;" app:layout_constraintStart_toEndOf="&amp;CHAR(34)&amp;"@+id/"&amp;K2&amp;CHAR(34)&amp;" app:layout_constraintTop_toBottomOf="&amp;CHAR(34)&amp;"@id/"&amp;L1&amp;CHAR(34)&amp;" /&gt;"</f>
-        <v>&lt;Button android:id="@+id/button22" android:layout_width="wrap_content" android:layout_height="wrap_content" android:minWidth="40dp" android:text="O" app:layout_constraintEnd_toStartOf="@id/button23" app:layout_constraintHorizontal_weight="1" app:layout_constraintStart_toEndOf="@+id/button21" app:layout_constraintTop_toBottomOf="@id/button12" /&gt;</v>
-      </c>
-      <c r="M12" t="str">
-        <f t="shared" ref="M12:R12" si="11">"&lt;Button android:id="&amp;CHAR(34)&amp;"@+id/"&amp;M2&amp;CHAR(34)&amp;" android:layout_width="&amp;CHAR(34)&amp;"wrap_content"&amp;CHAR(34)&amp;" android:layout_height="&amp;CHAR(34)&amp;"wrap_content"&amp;CHAR(34)&amp;" android:minWidth="&amp;CHAR(34)&amp;"40dp"&amp;CHAR(34)&amp;" android:text="&amp;CHAR(34)&amp;"O"&amp;CHAR(34)&amp;" app:layout_constraintEnd_toStartOf="&amp;CHAR(34)&amp;"@id/"&amp;N2&amp;CHAR(34)&amp;" app:layout_constraintHorizontal_weight="&amp;CHAR(34)&amp;"1"&amp;CHAR(34)&amp;" app:layout_constraintStart_toEndOf="&amp;CHAR(34)&amp;"@+id/"&amp;L2&amp;CHAR(34)&amp;" app:layout_constraintTop_toBottomOf="&amp;CHAR(34)&amp;"@id/"&amp;M1&amp;CHAR(34)&amp;" /&gt;"</f>
-        <v>&lt;Button android:id="@+id/button23" android:layout_width="wrap_content" android:layout_height="wrap_content" android:minWidth="40dp" android:text="O" app:layout_constraintEnd_toStartOf="@id/button24" app:layout_constraintHorizontal_weight="1" app:layout_constraintStart_toEndOf="@+id/button22" app:layout_constraintTop_toBottomOf="@id/button13" /&gt;</v>
-      </c>
-      <c r="N12" t="str">
+        <f>"&lt;Button android:id="&amp;CHAR(34)&amp;"@+id/"&amp;K2&amp;CHAR(34)&amp;" android:layout_width="&amp;CHAR(34)&amp;"wrap_content"&amp;CHAR(34)&amp;" android:layout_height="&amp;CHAR(34)&amp;"wrap_content"&amp;CHAR(34)&amp;" android:layout_marginLeft="&amp;CHAR(34)&amp;"8dp"&amp;CHAR(34)&amp;" android:layout_marginStart="&amp;CHAR(34)&amp;"8dp"&amp;CHAR(34)&amp;" android:minWidth="&amp;CHAR(34)&amp;"40dp"&amp;CHAR(34)&amp;" android:onClick="&amp;CHAR(34)&amp;K2&amp;CHAR(34)&amp;" app:layout_constraintEnd_toStartOf="&amp;CHAR(34)&amp;"@id/"&amp;L2&amp;CHAR(34)&amp;" app:layout_constraintHorizontal_weight="&amp;CHAR(34)&amp;"1"&amp;CHAR(34)&amp;" app:layout_constraintStart_toStartOf="&amp;CHAR(34)&amp;"parent"&amp;CHAR(34)&amp;" app:layout_constraintTop_toBottomOf="&amp;CHAR(34)&amp;"@id/"&amp;K1&amp;CHAR(34)&amp;" /&gt;"</f>
+        <v>&lt;Button android:id="@+id/button21" android:layout_width="wrap_content" android:layout_height="wrap_content" android:layout_marginLeft="8dp" android:layout_marginStart="8dp" android:minWidth="40dp" android:onClick="button21" app:layout_constraintEnd_toStartOf="@id/button22" app:layout_constraintHorizontal_weight="1" app:layout_constraintStart_toStartOf="parent" app:layout_constraintTop_toBottomOf="@id/button11" /&gt;</v>
+      </c>
+      <c r="L12" s="6" t="str">
+        <f>"&lt;Button android:id="&amp;CHAR(34)&amp;"@+id/"&amp;L2&amp;CHAR(34)&amp;" android:layout_width="&amp;CHAR(34)&amp;"wrap_content"&amp;CHAR(34)&amp;" android:layout_height="&amp;CHAR(34)&amp;"wrap_content"&amp;CHAR(34)&amp;" android:minWidth="&amp;CHAR(34)&amp;"40dp"&amp;CHAR(34)&amp;" android:onClick="&amp;CHAR(34)&amp;L2&amp;CHAR(34)&amp;" app:layout_constraintEnd_toStartOf="&amp;CHAR(34)&amp;"@id/"&amp;M2&amp;CHAR(34)&amp;" app:layout_constraintHorizontal_weight="&amp;CHAR(34)&amp;"1"&amp;CHAR(34)&amp;" app:layout_constraintStart_toEndOf="&amp;CHAR(34)&amp;"@+id/"&amp;K2&amp;CHAR(34)&amp;" app:layout_constraintTop_toBottomOf="&amp;CHAR(34)&amp;"@id/"&amp;L1&amp;CHAR(34)&amp;" /&gt;"</f>
+        <v>&lt;Button android:id="@+id/button22" android:layout_width="wrap_content" android:layout_height="wrap_content" android:minWidth="40dp" android:onClick="button22" app:layout_constraintEnd_toStartOf="@id/button23" app:layout_constraintHorizontal_weight="1" app:layout_constraintStart_toEndOf="@+id/button21" app:layout_constraintTop_toBottomOf="@id/button12" /&gt;</v>
+      </c>
+      <c r="M12" s="6" t="str">
+        <f t="shared" ref="M12:R12" si="11">"&lt;Button android:id="&amp;CHAR(34)&amp;"@+id/"&amp;M2&amp;CHAR(34)&amp;" android:layout_width="&amp;CHAR(34)&amp;"wrap_content"&amp;CHAR(34)&amp;" android:layout_height="&amp;CHAR(34)&amp;"wrap_content"&amp;CHAR(34)&amp;" android:minWidth="&amp;CHAR(34)&amp;"40dp"&amp;CHAR(34)&amp;" android:onClick="&amp;CHAR(34)&amp;M2&amp;CHAR(34)&amp;" app:layout_constraintEnd_toStartOf="&amp;CHAR(34)&amp;"@id/"&amp;N2&amp;CHAR(34)&amp;" app:layout_constraintHorizontal_weight="&amp;CHAR(34)&amp;"1"&amp;CHAR(34)&amp;" app:layout_constraintStart_toEndOf="&amp;CHAR(34)&amp;"@+id/"&amp;L2&amp;CHAR(34)&amp;" app:layout_constraintTop_toBottomOf="&amp;CHAR(34)&amp;"@id/"&amp;M1&amp;CHAR(34)&amp;" /&gt;"</f>
+        <v>&lt;Button android:id="@+id/button23" android:layout_width="wrap_content" android:layout_height="wrap_content" android:minWidth="40dp" android:onClick="button23" app:layout_constraintEnd_toStartOf="@id/button24" app:layout_constraintHorizontal_weight="1" app:layout_constraintStart_toEndOf="@+id/button22" app:layout_constraintTop_toBottomOf="@id/button13" /&gt;</v>
+      </c>
+      <c r="N12" s="6" t="str">
         <f t="shared" si="11"/>
-        <v>&lt;Button android:id="@+id/button24" android:layout_width="wrap_content" android:layout_height="wrap_content" android:minWidth="40dp" android:text="O" app:layout_constraintEnd_toStartOf="@id/button25" app:layout_constraintHorizontal_weight="1" app:layout_constraintStart_toEndOf="@+id/button23" app:layout_constraintTop_toBottomOf="@id/button14" /&gt;</v>
-      </c>
-      <c r="O12" t="str">
+        <v>&lt;Button android:id="@+id/button24" android:layout_width="wrap_content" android:layout_height="wrap_content" android:minWidth="40dp" android:onClick="button24" app:layout_constraintEnd_toStartOf="@id/button25" app:layout_constraintHorizontal_weight="1" app:layout_constraintStart_toEndOf="@+id/button23" app:layout_constraintTop_toBottomOf="@id/button14" /&gt;</v>
+      </c>
+      <c r="O12" s="6" t="str">
         <f t="shared" si="11"/>
-        <v>&lt;Button android:id="@+id/button25" android:layout_width="wrap_content" android:layout_height="wrap_content" android:minWidth="40dp" android:text="O" app:layout_constraintEnd_toStartOf="@id/button26" app:layout_constraintHorizontal_weight="1" app:layout_constraintStart_toEndOf="@+id/button24" app:layout_constraintTop_toBottomOf="@id/button15" /&gt;</v>
-      </c>
-      <c r="P12" t="str">
+        <v>&lt;Button android:id="@+id/button25" android:layout_width="wrap_content" android:layout_height="wrap_content" android:minWidth="40dp" android:onClick="button25" app:layout_constraintEnd_toStartOf="@id/button26" app:layout_constraintHorizontal_weight="1" app:layout_constraintStart_toEndOf="@+id/button24" app:layout_constraintTop_toBottomOf="@id/button15" /&gt;</v>
+      </c>
+      <c r="P12" s="6" t="str">
         <f t="shared" si="11"/>
-        <v>&lt;Button android:id="@+id/button26" android:layout_width="wrap_content" android:layout_height="wrap_content" android:minWidth="40dp" android:text="O" app:layout_constraintEnd_toStartOf="@id/button27" app:layout_constraintHorizontal_weight="1" app:layout_constraintStart_toEndOf="@+id/button25" app:layout_constraintTop_toBottomOf="@id/button16" /&gt;</v>
-      </c>
-      <c r="Q12" t="str">
+        <v>&lt;Button android:id="@+id/button26" android:layout_width="wrap_content" android:layout_height="wrap_content" android:minWidth="40dp" android:onClick="button26" app:layout_constraintEnd_toStartOf="@id/button27" app:layout_constraintHorizontal_weight="1" app:layout_constraintStart_toEndOf="@+id/button25" app:layout_constraintTop_toBottomOf="@id/button16" /&gt;</v>
+      </c>
+      <c r="Q12" s="6" t="str">
         <f t="shared" si="11"/>
-        <v>&lt;Button android:id="@+id/button27" android:layout_width="wrap_content" android:layout_height="wrap_content" android:minWidth="40dp" android:text="O" app:layout_constraintEnd_toStartOf="@id/button28" app:layout_constraintHorizontal_weight="1" app:layout_constraintStart_toEndOf="@+id/button26" app:layout_constraintTop_toBottomOf="@id/button17" /&gt;</v>
-      </c>
-      <c r="R12" t="str">
+        <v>&lt;Button android:id="@+id/button27" android:layout_width="wrap_content" android:layout_height="wrap_content" android:minWidth="40dp" android:onClick="button27" app:layout_constraintEnd_toStartOf="@id/button28" app:layout_constraintHorizontal_weight="1" app:layout_constraintStart_toEndOf="@+id/button26" app:layout_constraintTop_toBottomOf="@id/button17" /&gt;</v>
+      </c>
+      <c r="R12" s="6" t="str">
         <f t="shared" si="11"/>
-        <v>&lt;Button android:id="@+id/button28" android:layout_width="wrap_content" android:layout_height="wrap_content" android:minWidth="40dp" android:text="O" app:layout_constraintEnd_toStartOf="@id/button29" app:layout_constraintHorizontal_weight="1" app:layout_constraintStart_toEndOf="@+id/button27" app:layout_constraintTop_toBottomOf="@id/button18" /&gt;</v>
-      </c>
-      <c r="S12" s="4" t="str">
-        <f>"&lt;Button android:id="&amp;CHAR(34)&amp;"@+id/"&amp;S2&amp;CHAR(34)&amp;" android:layout_width="&amp;CHAR(34)&amp;"wrap_content"&amp;CHAR(34)&amp;" android:layout_height="&amp;CHAR(34)&amp;"wrap_content"&amp;CHAR(34)&amp;" android:layout_marginEnd="&amp;CHAR(34)&amp;"8dp"&amp;CHAR(34)&amp;" android:layout_marginRight="&amp;CHAR(34)&amp;"8dp"&amp;CHAR(34)&amp;" android:minWidth="&amp;CHAR(34)&amp;"40dp"&amp;CHAR(34)&amp;" android:text="&amp;CHAR(34)&amp;"O"&amp;CHAR(34)&amp;" app:layout_constraintEnd_toEndOf="&amp;CHAR(34)&amp;"parent"&amp;CHAR(34)&amp;" app:layout_constraintHorizontal_weight="&amp;CHAR(34)&amp;"1"&amp;CHAR(34)&amp;" app:layout_constraintStart_toEndOf="&amp;CHAR(34)&amp;"@id/"&amp;R2&amp;CHAR(34)&amp;" app:layout_constraintTop_toBottomOf="&amp;CHAR(34)&amp;"@id/"&amp;S1&amp;CHAR(34)&amp;" /&gt;"</f>
-        <v>&lt;Button android:id="@+id/button29" android:layout_width="wrap_content" android:layout_height="wrap_content" android:layout_marginEnd="8dp" android:layout_marginRight="8dp" android:minWidth="40dp" android:text="O" app:layout_constraintEnd_toEndOf="parent" app:layout_constraintHorizontal_weight="1" app:layout_constraintStart_toEndOf="@id/button28" app:layout_constraintTop_toBottomOf="@id/button19" /&gt;</v>
+        <v>&lt;Button android:id="@+id/button28" android:layout_width="wrap_content" android:layout_height="wrap_content" android:minWidth="40dp" android:onClick="button28" app:layout_constraintEnd_toStartOf="@id/button29" app:layout_constraintHorizontal_weight="1" app:layout_constraintStart_toEndOf="@+id/button27" app:layout_constraintTop_toBottomOf="@id/button18" /&gt;</v>
+      </c>
+      <c r="S12" s="8" t="str">
+        <f>"&lt;Button android:id="&amp;CHAR(34)&amp;"@+id/"&amp;S2&amp;CHAR(34)&amp;" android:layout_width="&amp;CHAR(34)&amp;"wrap_content"&amp;CHAR(34)&amp;" android:layout_height="&amp;CHAR(34)&amp;"wrap_content"&amp;CHAR(34)&amp;" android:layout_marginEnd="&amp;CHAR(34)&amp;"8dp"&amp;CHAR(34)&amp;" android:layout_marginRight="&amp;CHAR(34)&amp;"8dp"&amp;CHAR(34)&amp;" android:minWidth="&amp;CHAR(34)&amp;"40dp"&amp;CHAR(34)&amp;" android:onClick="&amp;CHAR(34)&amp;S2&amp;CHAR(34)&amp;" app:layout_constraintEnd_toEndOf="&amp;CHAR(34)&amp;"parent"&amp;CHAR(34)&amp;" app:layout_constraintHorizontal_weight="&amp;CHAR(34)&amp;"1"&amp;CHAR(34)&amp;" app:layout_constraintStart_toEndOf="&amp;CHAR(34)&amp;"@id/"&amp;R2&amp;CHAR(34)&amp;" app:layout_constraintTop_toBottomOf="&amp;CHAR(34)&amp;"@id/"&amp;S1&amp;CHAR(34)&amp;" /&gt;"</f>
+        <v>&lt;Button android:id="@+id/button29" android:layout_width="wrap_content" android:layout_height="wrap_content" android:layout_marginEnd="8dp" android:layout_marginRight="8dp" android:minWidth="40dp" android:onClick="button29" app:layout_constraintEnd_toEndOf="parent" app:layout_constraintHorizontal_weight="1" app:layout_constraintStart_toEndOf="@id/button28" app:layout_constraintTop_toBottomOf="@id/button19" /&gt;</v>
       </c>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="K13" s="4" t="str">
-        <f t="shared" ref="K13:K19" si="12">"&lt;Button android:id="&amp;CHAR(34)&amp;"@+id/"&amp;K3&amp;CHAR(34)&amp;" android:layout_width="&amp;CHAR(34)&amp;"wrap_content"&amp;CHAR(34)&amp;" android:layout_height="&amp;CHAR(34)&amp;"wrap_content"&amp;CHAR(34)&amp;" android:layout_marginLeft="&amp;CHAR(34)&amp;"8dp"&amp;CHAR(34)&amp;" android:layout_marginStart="&amp;CHAR(34)&amp;"8dp"&amp;CHAR(34)&amp;" android:minWidth="&amp;CHAR(34)&amp;"40dp"&amp;CHAR(34)&amp;" android:text="&amp;CHAR(34)&amp;"O"&amp;CHAR(34)&amp;" app:layout_constraintEnd_toStartOf="&amp;CHAR(34)&amp;"@id/"&amp;L3&amp;CHAR(34)&amp;" app:layout_constraintHorizontal_weight="&amp;CHAR(34)&amp;"1"&amp;CHAR(34)&amp;" app:layout_constraintStart_toStartOf="&amp;CHAR(34)&amp;"parent"&amp;CHAR(34)&amp;" app:layout_constraintTop_toBottomOf="&amp;CHAR(34)&amp;"@id/"&amp;K2&amp;CHAR(34)&amp;" /&gt;"</f>
-        <v>&lt;Button android:id="@+id/button31" android:layout_width="wrap_content" android:layout_height="wrap_content" android:layout_marginLeft="8dp" android:layout_marginStart="8dp" android:minWidth="40dp" android:text="O" app:layout_constraintEnd_toStartOf="@id/button32" app:layout_constraintHorizontal_weight="1" app:layout_constraintStart_toStartOf="parent" app:layout_constraintTop_toBottomOf="@id/button21" /&gt;</v>
-      </c>
-      <c r="L13" t="str">
-        <f t="shared" ref="L13:R13" si="13">"&lt;Button android:id="&amp;CHAR(34)&amp;"@+id/"&amp;L3&amp;CHAR(34)&amp;" android:layout_width="&amp;CHAR(34)&amp;"wrap_content"&amp;CHAR(34)&amp;" android:layout_height="&amp;CHAR(34)&amp;"wrap_content"&amp;CHAR(34)&amp;" android:minWidth="&amp;CHAR(34)&amp;"40dp"&amp;CHAR(34)&amp;" android:text="&amp;CHAR(34)&amp;"O"&amp;CHAR(34)&amp;" app:layout_constraintEnd_toStartOf="&amp;CHAR(34)&amp;"@id/"&amp;M3&amp;CHAR(34)&amp;" app:layout_constraintHorizontal_weight="&amp;CHAR(34)&amp;"1"&amp;CHAR(34)&amp;" app:layout_constraintStart_toEndOf="&amp;CHAR(34)&amp;"@+id/"&amp;K3&amp;CHAR(34)&amp;" app:layout_constraintTop_toBottomOf="&amp;CHAR(34)&amp;"@id/"&amp;L2&amp;CHAR(34)&amp;" /&gt;"</f>
-        <v>&lt;Button android:id="@+id/button32" android:layout_width="wrap_content" android:layout_height="wrap_content" android:minWidth="40dp" android:text="O" app:layout_constraintEnd_toStartOf="@id/button33" app:layout_constraintHorizontal_weight="1" app:layout_constraintStart_toEndOf="@+id/button31" app:layout_constraintTop_toBottomOf="@id/button22" /&gt;</v>
-      </c>
-      <c r="M13" t="str">
-        <f t="shared" si="13"/>
-        <v>&lt;Button android:id="@+id/button33" android:layout_width="wrap_content" android:layout_height="wrap_content" android:minWidth="40dp" android:text="O" app:layout_constraintEnd_toStartOf="@id/button34" app:layout_constraintHorizontal_weight="1" app:layout_constraintStart_toEndOf="@+id/button32" app:layout_constraintTop_toBottomOf="@id/button23" /&gt;</v>
-      </c>
-      <c r="N13" t="str">
-        <f t="shared" si="13"/>
-        <v>&lt;Button android:id="@+id/button34" android:layout_width="wrap_content" android:layout_height="wrap_content" android:minWidth="40dp" android:text="O" app:layout_constraintEnd_toStartOf="@id/button35" app:layout_constraintHorizontal_weight="1" app:layout_constraintStart_toEndOf="@+id/button33" app:layout_constraintTop_toBottomOf="@id/button24" /&gt;</v>
-      </c>
-      <c r="O13" t="str">
-        <f t="shared" si="13"/>
-        <v>&lt;Button android:id="@+id/button35" android:layout_width="wrap_content" android:layout_height="wrap_content" android:minWidth="40dp" android:text="O" app:layout_constraintEnd_toStartOf="@id/button36" app:layout_constraintHorizontal_weight="1" app:layout_constraintStart_toEndOf="@+id/button34" app:layout_constraintTop_toBottomOf="@id/button25" /&gt;</v>
-      </c>
-      <c r="P13" t="str">
-        <f t="shared" si="13"/>
-        <v>&lt;Button android:id="@+id/button36" android:layout_width="wrap_content" android:layout_height="wrap_content" android:minWidth="40dp" android:text="O" app:layout_constraintEnd_toStartOf="@id/button37" app:layout_constraintHorizontal_weight="1" app:layout_constraintStart_toEndOf="@+id/button35" app:layout_constraintTop_toBottomOf="@id/button26" /&gt;</v>
-      </c>
-      <c r="Q13" t="str">
-        <f t="shared" si="13"/>
-        <v>&lt;Button android:id="@+id/button37" android:layout_width="wrap_content" android:layout_height="wrap_content" android:minWidth="40dp" android:text="O" app:layout_constraintEnd_toStartOf="@id/button38" app:layout_constraintHorizontal_weight="1" app:layout_constraintStart_toEndOf="@+id/button36" app:layout_constraintTop_toBottomOf="@id/button27" /&gt;</v>
-      </c>
-      <c r="R13" t="str">
-        <f t="shared" si="13"/>
-        <v>&lt;Button android:id="@+id/button38" android:layout_width="wrap_content" android:layout_height="wrap_content" android:minWidth="40dp" android:text="O" app:layout_constraintEnd_toStartOf="@id/button39" app:layout_constraintHorizontal_weight="1" app:layout_constraintStart_toEndOf="@+id/button37" app:layout_constraintTop_toBottomOf="@id/button28" /&gt;</v>
-      </c>
-      <c r="S13" s="4" t="str">
-        <f t="shared" ref="S13:S19" si="14">"&lt;Button android:id="&amp;CHAR(34)&amp;"@+id/"&amp;S3&amp;CHAR(34)&amp;" android:layout_width="&amp;CHAR(34)&amp;"wrap_content"&amp;CHAR(34)&amp;" android:layout_height="&amp;CHAR(34)&amp;"wrap_content"&amp;CHAR(34)&amp;" android:layout_marginEnd="&amp;CHAR(34)&amp;"8dp"&amp;CHAR(34)&amp;" android:layout_marginRight="&amp;CHAR(34)&amp;"8dp"&amp;CHAR(34)&amp;" android:minWidth="&amp;CHAR(34)&amp;"40dp"&amp;CHAR(34)&amp;" android:text="&amp;CHAR(34)&amp;"O"&amp;CHAR(34)&amp;" app:layout_constraintEnd_toEndOf="&amp;CHAR(34)&amp;"parent"&amp;CHAR(34)&amp;" app:layout_constraintHorizontal_weight="&amp;CHAR(34)&amp;"1"&amp;CHAR(34)&amp;" app:layout_constraintStart_toEndOf="&amp;CHAR(34)&amp;"@id/"&amp;R3&amp;CHAR(34)&amp;" app:layout_constraintTop_toBottomOf="&amp;CHAR(34)&amp;"@id/"&amp;S2&amp;CHAR(34)&amp;" /&gt;"</f>
-        <v>&lt;Button android:id="@+id/button39" android:layout_width="wrap_content" android:layout_height="wrap_content" android:layout_marginEnd="8dp" android:layout_marginRight="8dp" android:minWidth="40dp" android:text="O" app:layout_constraintEnd_toEndOf="parent" app:layout_constraintHorizontal_weight="1" app:layout_constraintStart_toEndOf="@id/button38" app:layout_constraintTop_toBottomOf="@id/button29" /&gt;</v>
+        <f t="shared" ref="K13:K19" si="12">"&lt;Button android:id="&amp;CHAR(34)&amp;"@+id/"&amp;K3&amp;CHAR(34)&amp;" android:layout_width="&amp;CHAR(34)&amp;"wrap_content"&amp;CHAR(34)&amp;" android:layout_height="&amp;CHAR(34)&amp;"wrap_content"&amp;CHAR(34)&amp;" android:layout_marginLeft="&amp;CHAR(34)&amp;"8dp"&amp;CHAR(34)&amp;" android:layout_marginStart="&amp;CHAR(34)&amp;"8dp"&amp;CHAR(34)&amp;" android:minWidth="&amp;CHAR(34)&amp;"40dp"&amp;CHAR(34)&amp;" android:onClick="&amp;CHAR(34)&amp;K3&amp;CHAR(34)&amp;" app:layout_constraintEnd_toStartOf="&amp;CHAR(34)&amp;"@id/"&amp;L3&amp;CHAR(34)&amp;" app:layout_constraintHorizontal_weight="&amp;CHAR(34)&amp;"1"&amp;CHAR(34)&amp;" app:layout_constraintStart_toStartOf="&amp;CHAR(34)&amp;"parent"&amp;CHAR(34)&amp;" app:layout_constraintTop_toBottomOf="&amp;CHAR(34)&amp;"@id/"&amp;K2&amp;CHAR(34)&amp;" /&gt;"</f>
+        <v>&lt;Button android:id="@+id/button31" android:layout_width="wrap_content" android:layout_height="wrap_content" android:layout_marginLeft="8dp" android:layout_marginStart="8dp" android:minWidth="40dp" android:onClick="button31" app:layout_constraintEnd_toStartOf="@id/button32" app:layout_constraintHorizontal_weight="1" app:layout_constraintStart_toStartOf="parent" app:layout_constraintTop_toBottomOf="@id/button21" /&gt;</v>
+      </c>
+      <c r="L13" s="6" t="str">
+        <f t="shared" ref="L13:R19" si="13">"&lt;Button android:id="&amp;CHAR(34)&amp;"@+id/"&amp;L3&amp;CHAR(34)&amp;" android:layout_width="&amp;CHAR(34)&amp;"wrap_content"&amp;CHAR(34)&amp;" android:layout_height="&amp;CHAR(34)&amp;"wrap_content"&amp;CHAR(34)&amp;" android:minWidth="&amp;CHAR(34)&amp;"40dp"&amp;CHAR(34)&amp;" android:onClick="&amp;CHAR(34)&amp;L3&amp;CHAR(34)&amp;" app:layout_constraintEnd_toStartOf="&amp;CHAR(34)&amp;"@id/"&amp;M3&amp;CHAR(34)&amp;" app:layout_constraintHorizontal_weight="&amp;CHAR(34)&amp;"1"&amp;CHAR(34)&amp;" app:layout_constraintStart_toEndOf="&amp;CHAR(34)&amp;"@+id/"&amp;K3&amp;CHAR(34)&amp;" app:layout_constraintTop_toBottomOf="&amp;CHAR(34)&amp;"@id/"&amp;L2&amp;CHAR(34)&amp;" /&gt;"</f>
+        <v>&lt;Button android:id="@+id/button32" android:layout_width="wrap_content" android:layout_height="wrap_content" android:minWidth="40dp" android:onClick="button32" app:layout_constraintEnd_toStartOf="@id/button33" app:layout_constraintHorizontal_weight="1" app:layout_constraintStart_toEndOf="@+id/button31" app:layout_constraintTop_toBottomOf="@id/button22" /&gt;</v>
+      </c>
+      <c r="M13" s="6" t="str">
+        <f t="shared" si="13"/>
+        <v>&lt;Button android:id="@+id/button33" android:layout_width="wrap_content" android:layout_height="wrap_content" android:minWidth="40dp" android:onClick="button33" app:layout_constraintEnd_toStartOf="@id/button34" app:layout_constraintHorizontal_weight="1" app:layout_constraintStart_toEndOf="@+id/button32" app:layout_constraintTop_toBottomOf="@id/button23" /&gt;</v>
+      </c>
+      <c r="N13" s="6" t="str">
+        <f t="shared" si="13"/>
+        <v>&lt;Button android:id="@+id/button34" android:layout_width="wrap_content" android:layout_height="wrap_content" android:minWidth="40dp" android:onClick="button34" app:layout_constraintEnd_toStartOf="@id/button35" app:layout_constraintHorizontal_weight="1" app:layout_constraintStart_toEndOf="@+id/button33" app:layout_constraintTop_toBottomOf="@id/button24" /&gt;</v>
+      </c>
+      <c r="O13" s="6" t="str">
+        <f t="shared" si="13"/>
+        <v>&lt;Button android:id="@+id/button35" android:layout_width="wrap_content" android:layout_height="wrap_content" android:minWidth="40dp" android:onClick="button35" app:layout_constraintEnd_toStartOf="@id/button36" app:layout_constraintHorizontal_weight="1" app:layout_constraintStart_toEndOf="@+id/button34" app:layout_constraintTop_toBottomOf="@id/button25" /&gt;</v>
+      </c>
+      <c r="P13" s="6" t="str">
+        <f t="shared" si="13"/>
+        <v>&lt;Button android:id="@+id/button36" android:layout_width="wrap_content" android:layout_height="wrap_content" android:minWidth="40dp" android:onClick="button36" app:layout_constraintEnd_toStartOf="@id/button37" app:layout_constraintHorizontal_weight="1" app:layout_constraintStart_toEndOf="@+id/button35" app:layout_constraintTop_toBottomOf="@id/button26" /&gt;</v>
+      </c>
+      <c r="Q13" s="6" t="str">
+        <f t="shared" si="13"/>
+        <v>&lt;Button android:id="@+id/button37" android:layout_width="wrap_content" android:layout_height="wrap_content" android:minWidth="40dp" android:onClick="button37" app:layout_constraintEnd_toStartOf="@id/button38" app:layout_constraintHorizontal_weight="1" app:layout_constraintStart_toEndOf="@+id/button36" app:layout_constraintTop_toBottomOf="@id/button27" /&gt;</v>
+      </c>
+      <c r="R13" s="6" t="str">
+        <f t="shared" si="13"/>
+        <v>&lt;Button android:id="@+id/button38" android:layout_width="wrap_content" android:layout_height="wrap_content" android:minWidth="40dp" android:onClick="button38" app:layout_constraintEnd_toStartOf="@id/button39" app:layout_constraintHorizontal_weight="1" app:layout_constraintStart_toEndOf="@+id/button37" app:layout_constraintTop_toBottomOf="@id/button28" /&gt;</v>
+      </c>
+      <c r="S13" s="8" t="str">
+        <f t="shared" ref="S13:S19" si="14">"&lt;Button android:id="&amp;CHAR(34)&amp;"@+id/"&amp;S3&amp;CHAR(34)&amp;" android:layout_width="&amp;CHAR(34)&amp;"wrap_content"&amp;CHAR(34)&amp;" android:layout_height="&amp;CHAR(34)&amp;"wrap_content"&amp;CHAR(34)&amp;" android:layout_marginEnd="&amp;CHAR(34)&amp;"8dp"&amp;CHAR(34)&amp;" android:layout_marginRight="&amp;CHAR(34)&amp;"8dp"&amp;CHAR(34)&amp;" android:minWidth="&amp;CHAR(34)&amp;"40dp"&amp;CHAR(34)&amp;" android:onClick="&amp;CHAR(34)&amp;S3&amp;CHAR(34)&amp;" app:layout_constraintEnd_toEndOf="&amp;CHAR(34)&amp;"parent"&amp;CHAR(34)&amp;" app:layout_constraintHorizontal_weight="&amp;CHAR(34)&amp;"1"&amp;CHAR(34)&amp;" app:layout_constraintStart_toEndOf="&amp;CHAR(34)&amp;"@id/"&amp;R3&amp;CHAR(34)&amp;" app:layout_constraintTop_toBottomOf="&amp;CHAR(34)&amp;"@id/"&amp;S2&amp;CHAR(34)&amp;" /&gt;"</f>
+        <v>&lt;Button android:id="@+id/button39" android:layout_width="wrap_content" android:layout_height="wrap_content" android:layout_marginEnd="8dp" android:layout_marginRight="8dp" android:minWidth="40dp" android:onClick="button39" app:layout_constraintEnd_toEndOf="parent" app:layout_constraintHorizontal_weight="1" app:layout_constraintStart_toEndOf="@id/button38" app:layout_constraintTop_toBottomOf="@id/button29" /&gt;</v>
       </c>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="K14" s="4" t="str">
         <f t="shared" si="12"/>
-        <v>&lt;Button android:id="@+id/button41" android:layout_width="wrap_content" android:layout_height="wrap_content" android:layout_marginLeft="8dp" android:layout_marginStart="8dp" android:minWidth="40dp" android:text="O" app:layout_constraintEnd_toStartOf="@id/button42" app:layout_constraintHorizontal_weight="1" app:layout_constraintStart_toStartOf="parent" app:layout_constraintTop_toBottomOf="@id/button31" /&gt;</v>
-      </c>
-      <c r="L14" t="str">
-        <f t="shared" ref="L14:R14" si="15">"&lt;Button android:id="&amp;CHAR(34)&amp;"@+id/"&amp;L4&amp;CHAR(34)&amp;" android:layout_width="&amp;CHAR(34)&amp;"wrap_content"&amp;CHAR(34)&amp;" android:layout_height="&amp;CHAR(34)&amp;"wrap_content"&amp;CHAR(34)&amp;" android:minWidth="&amp;CHAR(34)&amp;"40dp"&amp;CHAR(34)&amp;" android:text="&amp;CHAR(34)&amp;"O"&amp;CHAR(34)&amp;" app:layout_constraintEnd_toStartOf="&amp;CHAR(34)&amp;"@id/"&amp;M4&amp;CHAR(34)&amp;" app:layout_constraintHorizontal_weight="&amp;CHAR(34)&amp;"1"&amp;CHAR(34)&amp;" app:layout_constraintStart_toEndOf="&amp;CHAR(34)&amp;"@+id/"&amp;K4&amp;CHAR(34)&amp;" app:layout_constraintTop_toBottomOf="&amp;CHAR(34)&amp;"@id/"&amp;L3&amp;CHAR(34)&amp;" /&gt;"</f>
-        <v>&lt;Button android:id="@+id/button42" android:layout_width="wrap_content" android:layout_height="wrap_content" android:minWidth="40dp" android:text="O" app:layout_constraintEnd_toStartOf="@id/button43" app:layout_constraintHorizontal_weight="1" app:layout_constraintStart_toEndOf="@+id/button41" app:layout_constraintTop_toBottomOf="@id/button32" /&gt;</v>
-      </c>
-      <c r="M14" t="str">
-        <f t="shared" si="15"/>
-        <v>&lt;Button android:id="@+id/button43" android:layout_width="wrap_content" android:layout_height="wrap_content" android:minWidth="40dp" android:text="O" app:layout_constraintEnd_toStartOf="@id/button44" app:layout_constraintHorizontal_weight="1" app:layout_constraintStart_toEndOf="@+id/button42" app:layout_constraintTop_toBottomOf="@id/button33" /&gt;</v>
-      </c>
-      <c r="N14" t="str">
-        <f t="shared" si="15"/>
-        <v>&lt;Button android:id="@+id/button44" android:layout_width="wrap_content" android:layout_height="wrap_content" android:minWidth="40dp" android:text="O" app:layout_constraintEnd_toStartOf="@id/button45" app:layout_constraintHorizontal_weight="1" app:layout_constraintStart_toEndOf="@+id/button43" app:layout_constraintTop_toBottomOf="@id/button34" /&gt;</v>
-      </c>
-      <c r="O14" t="str">
-        <f t="shared" si="15"/>
-        <v>&lt;Button android:id="@+id/button45" android:layout_width="wrap_content" android:layout_height="wrap_content" android:minWidth="40dp" android:text="O" app:layout_constraintEnd_toStartOf="@id/button46" app:layout_constraintHorizontal_weight="1" app:layout_constraintStart_toEndOf="@+id/button44" app:layout_constraintTop_toBottomOf="@id/button35" /&gt;</v>
-      </c>
-      <c r="P14" t="str">
-        <f t="shared" si="15"/>
-        <v>&lt;Button android:id="@+id/button46" android:layout_width="wrap_content" android:layout_height="wrap_content" android:minWidth="40dp" android:text="O" app:layout_constraintEnd_toStartOf="@id/button47" app:layout_constraintHorizontal_weight="1" app:layout_constraintStart_toEndOf="@+id/button45" app:layout_constraintTop_toBottomOf="@id/button36" /&gt;</v>
-      </c>
-      <c r="Q14" t="str">
-        <f t="shared" si="15"/>
-        <v>&lt;Button android:id="@+id/button47" android:layout_width="wrap_content" android:layout_height="wrap_content" android:minWidth="40dp" android:text="O" app:layout_constraintEnd_toStartOf="@id/button48" app:layout_constraintHorizontal_weight="1" app:layout_constraintStart_toEndOf="@+id/button46" app:layout_constraintTop_toBottomOf="@id/button37" /&gt;</v>
-      </c>
-      <c r="R14" t="str">
-        <f t="shared" si="15"/>
-        <v>&lt;Button android:id="@+id/button48" android:layout_width="wrap_content" android:layout_height="wrap_content" android:minWidth="40dp" android:text="O" app:layout_constraintEnd_toStartOf="@id/button49" app:layout_constraintHorizontal_weight="1" app:layout_constraintStart_toEndOf="@+id/button47" app:layout_constraintTop_toBottomOf="@id/button38" /&gt;</v>
-      </c>
-      <c r="S14" s="4" t="str">
+        <v>&lt;Button android:id="@+id/button41" android:layout_width="wrap_content" android:layout_height="wrap_content" android:layout_marginLeft="8dp" android:layout_marginStart="8dp" android:minWidth="40dp" android:onClick="button41" app:layout_constraintEnd_toStartOf="@id/button42" app:layout_constraintHorizontal_weight="1" app:layout_constraintStart_toStartOf="parent" app:layout_constraintTop_toBottomOf="@id/button31" /&gt;</v>
+      </c>
+      <c r="L14" s="6" t="str">
+        <f t="shared" si="13"/>
+        <v>&lt;Button android:id="@+id/button42" android:layout_width="wrap_content" android:layout_height="wrap_content" android:minWidth="40dp" android:onClick="button42" app:layout_constraintEnd_toStartOf="@id/button43" app:layout_constraintHorizontal_weight="1" app:layout_constraintStart_toEndOf="@+id/button41" app:layout_constraintTop_toBottomOf="@id/button32" /&gt;</v>
+      </c>
+      <c r="M14" s="6" t="str">
+        <f t="shared" si="13"/>
+        <v>&lt;Button android:id="@+id/button43" android:layout_width="wrap_content" android:layout_height="wrap_content" android:minWidth="40dp" android:onClick="button43" app:layout_constraintEnd_toStartOf="@id/button44" app:layout_constraintHorizontal_weight="1" app:layout_constraintStart_toEndOf="@+id/button42" app:layout_constraintTop_toBottomOf="@id/button33" /&gt;</v>
+      </c>
+      <c r="N14" s="6" t="str">
+        <f t="shared" si="13"/>
+        <v>&lt;Button android:id="@+id/button44" android:layout_width="wrap_content" android:layout_height="wrap_content" android:minWidth="40dp" android:onClick="button44" app:layout_constraintEnd_toStartOf="@id/button45" app:layout_constraintHorizontal_weight="1" app:layout_constraintStart_toEndOf="@+id/button43" app:layout_constraintTop_toBottomOf="@id/button34" /&gt;</v>
+      </c>
+      <c r="O14" s="6" t="str">
+        <f t="shared" si="13"/>
+        <v>&lt;Button android:id="@+id/button45" android:layout_width="wrap_content" android:layout_height="wrap_content" android:minWidth="40dp" android:onClick="button45" app:layout_constraintEnd_toStartOf="@id/button46" app:layout_constraintHorizontal_weight="1" app:layout_constraintStart_toEndOf="@+id/button44" app:layout_constraintTop_toBottomOf="@id/button35" /&gt;</v>
+      </c>
+      <c r="P14" s="6" t="str">
+        <f t="shared" si="13"/>
+        <v>&lt;Button android:id="@+id/button46" android:layout_width="wrap_content" android:layout_height="wrap_content" android:minWidth="40dp" android:onClick="button46" app:layout_constraintEnd_toStartOf="@id/button47" app:layout_constraintHorizontal_weight="1" app:layout_constraintStart_toEndOf="@+id/button45" app:layout_constraintTop_toBottomOf="@id/button36" /&gt;</v>
+      </c>
+      <c r="Q14" s="6" t="str">
+        <f t="shared" si="13"/>
+        <v>&lt;Button android:id="@+id/button47" android:layout_width="wrap_content" android:layout_height="wrap_content" android:minWidth="40dp" android:onClick="button47" app:layout_constraintEnd_toStartOf="@id/button48" app:layout_constraintHorizontal_weight="1" app:layout_constraintStart_toEndOf="@+id/button46" app:layout_constraintTop_toBottomOf="@id/button37" /&gt;</v>
+      </c>
+      <c r="R14" s="6" t="str">
+        <f t="shared" si="13"/>
+        <v>&lt;Button android:id="@+id/button48" android:layout_width="wrap_content" android:layout_height="wrap_content" android:minWidth="40dp" android:onClick="button48" app:layout_constraintEnd_toStartOf="@id/button49" app:layout_constraintHorizontal_weight="1" app:layout_constraintStart_toEndOf="@+id/button47" app:layout_constraintTop_toBottomOf="@id/button38" /&gt;</v>
+      </c>
+      <c r="S14" s="8" t="str">
         <f t="shared" si="14"/>
-        <v>&lt;Button android:id="@+id/button49" android:layout_width="wrap_content" android:layout_height="wrap_content" android:layout_marginEnd="8dp" android:layout_marginRight="8dp" android:minWidth="40dp" android:text="O" app:layout_constraintEnd_toEndOf="parent" app:layout_constraintHorizontal_weight="1" app:layout_constraintStart_toEndOf="@id/button48" app:layout_constraintTop_toBottomOf="@id/button39" /&gt;</v>
+        <v>&lt;Button android:id="@+id/button49" android:layout_width="wrap_content" android:layout_height="wrap_content" android:layout_marginEnd="8dp" android:layout_marginRight="8dp" android:minWidth="40dp" android:onClick="button49" app:layout_constraintEnd_toEndOf="parent" app:layout_constraintHorizontal_weight="1" app:layout_constraintStart_toEndOf="@id/button48" app:layout_constraintTop_toBottomOf="@id/button39" /&gt;</v>
       </c>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.25">
       <c r="K15" s="4" t="str">
         <f t="shared" si="12"/>
-        <v>&lt;Button android:id="@+id/button51" android:layout_width="wrap_content" android:layout_height="wrap_content" android:layout_marginLeft="8dp" android:layout_marginStart="8dp" android:minWidth="40dp" android:text="O" app:layout_constraintEnd_toStartOf="@id/button52" app:layout_constraintHorizontal_weight="1" app:layout_constraintStart_toStartOf="parent" app:layout_constraintTop_toBottomOf="@id/button41" /&gt;</v>
-      </c>
-      <c r="L15" t="str">
-        <f t="shared" ref="L15:R15" si="16">"&lt;Button android:id="&amp;CHAR(34)&amp;"@+id/"&amp;L5&amp;CHAR(34)&amp;" android:layout_width="&amp;CHAR(34)&amp;"wrap_content"&amp;CHAR(34)&amp;" android:layout_height="&amp;CHAR(34)&amp;"wrap_content"&amp;CHAR(34)&amp;" android:minWidth="&amp;CHAR(34)&amp;"40dp"&amp;CHAR(34)&amp;" android:text="&amp;CHAR(34)&amp;"O"&amp;CHAR(34)&amp;" app:layout_constraintEnd_toStartOf="&amp;CHAR(34)&amp;"@id/"&amp;M5&amp;CHAR(34)&amp;" app:layout_constraintHorizontal_weight="&amp;CHAR(34)&amp;"1"&amp;CHAR(34)&amp;" app:layout_constraintStart_toEndOf="&amp;CHAR(34)&amp;"@+id/"&amp;K5&amp;CHAR(34)&amp;" app:layout_constraintTop_toBottomOf="&amp;CHAR(34)&amp;"@id/"&amp;L4&amp;CHAR(34)&amp;" /&gt;"</f>
-        <v>&lt;Button android:id="@+id/button52" android:layout_width="wrap_content" android:layout_height="wrap_content" android:minWidth="40dp" android:text="O" app:layout_constraintEnd_toStartOf="@id/button53" app:layout_constraintHorizontal_weight="1" app:layout_constraintStart_toEndOf="@+id/button51" app:layout_constraintTop_toBottomOf="@id/button42" /&gt;</v>
-      </c>
-      <c r="M15" t="str">
-        <f t="shared" si="16"/>
-        <v>&lt;Button android:id="@+id/button53" android:layout_width="wrap_content" android:layout_height="wrap_content" android:minWidth="40dp" android:text="O" app:layout_constraintEnd_toStartOf="@id/button54" app:layout_constraintHorizontal_weight="1" app:layout_constraintStart_toEndOf="@+id/button52" app:layout_constraintTop_toBottomOf="@id/button43" /&gt;</v>
-      </c>
-      <c r="N15" t="str">
-        <f t="shared" si="16"/>
-        <v>&lt;Button android:id="@+id/button54" android:layout_width="wrap_content" android:layout_height="wrap_content" android:minWidth="40dp" android:text="O" app:layout_constraintEnd_toStartOf="@id/button55" app:layout_constraintHorizontal_weight="1" app:layout_constraintStart_toEndOf="@+id/button53" app:layout_constraintTop_toBottomOf="@id/button44" /&gt;</v>
-      </c>
-      <c r="O15" t="str">
-        <f t="shared" si="16"/>
-        <v>&lt;Button android:id="@+id/button55" android:layout_width="wrap_content" android:layout_height="wrap_content" android:minWidth="40dp" android:text="O" app:layout_constraintEnd_toStartOf="@id/button56" app:layout_constraintHorizontal_weight="1" app:layout_constraintStart_toEndOf="@+id/button54" app:layout_constraintTop_toBottomOf="@id/button45" /&gt;</v>
-      </c>
-      <c r="P15" t="str">
-        <f t="shared" si="16"/>
-        <v>&lt;Button android:id="@+id/button56" android:layout_width="wrap_content" android:layout_height="wrap_content" android:minWidth="40dp" android:text="O" app:layout_constraintEnd_toStartOf="@id/button57" app:layout_constraintHorizontal_weight="1" app:layout_constraintStart_toEndOf="@+id/button55" app:layout_constraintTop_toBottomOf="@id/button46" /&gt;</v>
-      </c>
-      <c r="Q15" t="str">
-        <f t="shared" si="16"/>
-        <v>&lt;Button android:id="@+id/button57" android:layout_width="wrap_content" android:layout_height="wrap_content" android:minWidth="40dp" android:text="O" app:layout_constraintEnd_toStartOf="@id/button58" app:layout_constraintHorizontal_weight="1" app:layout_constraintStart_toEndOf="@+id/button56" app:layout_constraintTop_toBottomOf="@id/button47" /&gt;</v>
-      </c>
-      <c r="R15" t="str">
-        <f t="shared" si="16"/>
-        <v>&lt;Button android:id="@+id/button58" android:layout_width="wrap_content" android:layout_height="wrap_content" android:minWidth="40dp" android:text="O" app:layout_constraintEnd_toStartOf="@id/button59" app:layout_constraintHorizontal_weight="1" app:layout_constraintStart_toEndOf="@+id/button57" app:layout_constraintTop_toBottomOf="@id/button48" /&gt;</v>
-      </c>
-      <c r="S15" s="4" t="str">
+        <v>&lt;Button android:id="@+id/button51" android:layout_width="wrap_content" android:layout_height="wrap_content" android:layout_marginLeft="8dp" android:layout_marginStart="8dp" android:minWidth="40dp" android:onClick="button51" app:layout_constraintEnd_toStartOf="@id/button52" app:layout_constraintHorizontal_weight="1" app:layout_constraintStart_toStartOf="parent" app:layout_constraintTop_toBottomOf="@id/button41" /&gt;</v>
+      </c>
+      <c r="L15" s="6" t="str">
+        <f t="shared" si="13"/>
+        <v>&lt;Button android:id="@+id/button52" android:layout_width="wrap_content" android:layout_height="wrap_content" android:minWidth="40dp" android:onClick="button52" app:layout_constraintEnd_toStartOf="@id/button53" app:layout_constraintHorizontal_weight="1" app:layout_constraintStart_toEndOf="@+id/button51" app:layout_constraintTop_toBottomOf="@id/button42" /&gt;</v>
+      </c>
+      <c r="M15" s="6" t="str">
+        <f t="shared" si="13"/>
+        <v>&lt;Button android:id="@+id/button53" android:layout_width="wrap_content" android:layout_height="wrap_content" android:minWidth="40dp" android:onClick="button53" app:layout_constraintEnd_toStartOf="@id/button54" app:layout_constraintHorizontal_weight="1" app:layout_constraintStart_toEndOf="@+id/button52" app:layout_constraintTop_toBottomOf="@id/button43" /&gt;</v>
+      </c>
+      <c r="N15" s="6" t="str">
+        <f t="shared" si="13"/>
+        <v>&lt;Button android:id="@+id/button54" android:layout_width="wrap_content" android:layout_height="wrap_content" android:minWidth="40dp" android:onClick="button54" app:layout_constraintEnd_toStartOf="@id/button55" app:layout_constraintHorizontal_weight="1" app:layout_constraintStart_toEndOf="@+id/button53" app:layout_constraintTop_toBottomOf="@id/button44" /&gt;</v>
+      </c>
+      <c r="O15" s="6" t="str">
+        <f t="shared" si="13"/>
+        <v>&lt;Button android:id="@+id/button55" android:layout_width="wrap_content" android:layout_height="wrap_content" android:minWidth="40dp" android:onClick="button55" app:layout_constraintEnd_toStartOf="@id/button56" app:layout_constraintHorizontal_weight="1" app:layout_constraintStart_toEndOf="@+id/button54" app:layout_constraintTop_toBottomOf="@id/button45" /&gt;</v>
+      </c>
+      <c r="P15" s="6" t="str">
+        <f t="shared" si="13"/>
+        <v>&lt;Button android:id="@+id/button56" android:layout_width="wrap_content" android:layout_height="wrap_content" android:minWidth="40dp" android:onClick="button56" app:layout_constraintEnd_toStartOf="@id/button57" app:layout_constraintHorizontal_weight="1" app:layout_constraintStart_toEndOf="@+id/button55" app:layout_constraintTop_toBottomOf="@id/button46" /&gt;</v>
+      </c>
+      <c r="Q15" s="6" t="str">
+        <f t="shared" si="13"/>
+        <v>&lt;Button android:id="@+id/button57" android:layout_width="wrap_content" android:layout_height="wrap_content" android:minWidth="40dp" android:onClick="button57" app:layout_constraintEnd_toStartOf="@id/button58" app:layout_constraintHorizontal_weight="1" app:layout_constraintStart_toEndOf="@+id/button56" app:layout_constraintTop_toBottomOf="@id/button47" /&gt;</v>
+      </c>
+      <c r="R15" s="6" t="str">
+        <f t="shared" si="13"/>
+        <v>&lt;Button android:id="@+id/button58" android:layout_width="wrap_content" android:layout_height="wrap_content" android:minWidth="40dp" android:onClick="button58" app:layout_constraintEnd_toStartOf="@id/button59" app:layout_constraintHorizontal_weight="1" app:layout_constraintStart_toEndOf="@+id/button57" app:layout_constraintTop_toBottomOf="@id/button48" /&gt;</v>
+      </c>
+      <c r="S15" s="8" t="str">
         <f t="shared" si="14"/>
-        <v>&lt;Button android:id="@+id/button59" android:layout_width="wrap_content" android:layout_height="wrap_content" android:layout_marginEnd="8dp" android:layout_marginRight="8dp" android:minWidth="40dp" android:text="O" app:layout_constraintEnd_toEndOf="parent" app:layout_constraintHorizontal_weight="1" app:layout_constraintStart_toEndOf="@id/button58" app:layout_constraintTop_toBottomOf="@id/button49" /&gt;</v>
+        <v>&lt;Button android:id="@+id/button59" android:layout_width="wrap_content" android:layout_height="wrap_content" android:layout_marginEnd="8dp" android:layout_marginRight="8dp" android:minWidth="40dp" android:onClick="button59" app:layout_constraintEnd_toEndOf="parent" app:layout_constraintHorizontal_weight="1" app:layout_constraintStart_toEndOf="@id/button58" app:layout_constraintTop_toBottomOf="@id/button49" /&gt;</v>
       </c>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.25">
       <c r="K16" s="4" t="str">
         <f t="shared" si="12"/>
-        <v>&lt;Button android:id="@+id/button61" android:layout_width="wrap_content" android:layout_height="wrap_content" android:layout_marginLeft="8dp" android:layout_marginStart="8dp" android:minWidth="40dp" android:text="O" app:layout_constraintEnd_toStartOf="@id/button62" app:layout_constraintHorizontal_weight="1" app:layout_constraintStart_toStartOf="parent" app:layout_constraintTop_toBottomOf="@id/button51" /&gt;</v>
-      </c>
-      <c r="L16" t="str">
-        <f t="shared" ref="L16:R16" si="17">"&lt;Button android:id="&amp;CHAR(34)&amp;"@+id/"&amp;L6&amp;CHAR(34)&amp;" android:layout_width="&amp;CHAR(34)&amp;"wrap_content"&amp;CHAR(34)&amp;" android:layout_height="&amp;CHAR(34)&amp;"wrap_content"&amp;CHAR(34)&amp;" android:minWidth="&amp;CHAR(34)&amp;"40dp"&amp;CHAR(34)&amp;" android:text="&amp;CHAR(34)&amp;"O"&amp;CHAR(34)&amp;" app:layout_constraintEnd_toStartOf="&amp;CHAR(34)&amp;"@id/"&amp;M6&amp;CHAR(34)&amp;" app:layout_constraintHorizontal_weight="&amp;CHAR(34)&amp;"1"&amp;CHAR(34)&amp;" app:layout_constraintStart_toEndOf="&amp;CHAR(34)&amp;"@+id/"&amp;K6&amp;CHAR(34)&amp;" app:layout_constraintTop_toBottomOf="&amp;CHAR(34)&amp;"@id/"&amp;L5&amp;CHAR(34)&amp;" /&gt;"</f>
-        <v>&lt;Button android:id="@+id/button62" android:layout_width="wrap_content" android:layout_height="wrap_content" android:minWidth="40dp" android:text="O" app:layout_constraintEnd_toStartOf="@id/button63" app:layout_constraintHorizontal_weight="1" app:layout_constraintStart_toEndOf="@+id/button61" app:layout_constraintTop_toBottomOf="@id/button52" /&gt;</v>
-      </c>
-      <c r="M16" t="str">
-        <f t="shared" si="17"/>
-        <v>&lt;Button android:id="@+id/button63" android:layout_width="wrap_content" android:layout_height="wrap_content" android:minWidth="40dp" android:text="O" app:layout_constraintEnd_toStartOf="@id/button64" app:layout_constraintHorizontal_weight="1" app:layout_constraintStart_toEndOf="@+id/button62" app:layout_constraintTop_toBottomOf="@id/button53" /&gt;</v>
-      </c>
-      <c r="N16" t="str">
-        <f t="shared" si="17"/>
-        <v>&lt;Button android:id="@+id/button64" android:layout_width="wrap_content" android:layout_height="wrap_content" android:minWidth="40dp" android:text="O" app:layout_constraintEnd_toStartOf="@id/button65" app:layout_constraintHorizontal_weight="1" app:layout_constraintStart_toEndOf="@+id/button63" app:layout_constraintTop_toBottomOf="@id/button54" /&gt;</v>
-      </c>
-      <c r="O16" t="str">
-        <f t="shared" si="17"/>
-        <v>&lt;Button android:id="@+id/button65" android:layout_width="wrap_content" android:layout_height="wrap_content" android:minWidth="40dp" android:text="O" app:layout_constraintEnd_toStartOf="@id/button66" app:layout_constraintHorizontal_weight="1" app:layout_constraintStart_toEndOf="@+id/button64" app:layout_constraintTop_toBottomOf="@id/button55" /&gt;</v>
-      </c>
-      <c r="P16" t="str">
-        <f t="shared" si="17"/>
-        <v>&lt;Button android:id="@+id/button66" android:layout_width="wrap_content" android:layout_height="wrap_content" android:minWidth="40dp" android:text="O" app:layout_constraintEnd_toStartOf="@id/button67" app:layout_constraintHorizontal_weight="1" app:layout_constraintStart_toEndOf="@+id/button65" app:layout_constraintTop_toBottomOf="@id/button56" /&gt;</v>
-      </c>
-      <c r="Q16" t="str">
-        <f t="shared" si="17"/>
-        <v>&lt;Button android:id="@+id/button67" android:layout_width="wrap_content" android:layout_height="wrap_content" android:minWidth="40dp" android:text="O" app:layout_constraintEnd_toStartOf="@id/button68" app:layout_constraintHorizontal_weight="1" app:layout_constraintStart_toEndOf="@+id/button66" app:layout_constraintTop_toBottomOf="@id/button57" /&gt;</v>
-      </c>
-      <c r="R16" t="str">
-        <f t="shared" si="17"/>
-        <v>&lt;Button android:id="@+id/button68" android:layout_width="wrap_content" android:layout_height="wrap_content" android:minWidth="40dp" android:text="O" app:layout_constraintEnd_toStartOf="@id/button69" app:layout_constraintHorizontal_weight="1" app:layout_constraintStart_toEndOf="@+id/button67" app:layout_constraintTop_toBottomOf="@id/button58" /&gt;</v>
-      </c>
-      <c r="S16" s="4" t="str">
+        <v>&lt;Button android:id="@+id/button61" android:layout_width="wrap_content" android:layout_height="wrap_content" android:layout_marginLeft="8dp" android:layout_marginStart="8dp" android:minWidth="40dp" android:onClick="button61" app:layout_constraintEnd_toStartOf="@id/button62" app:layout_constraintHorizontal_weight="1" app:layout_constraintStart_toStartOf="parent" app:layout_constraintTop_toBottomOf="@id/button51" /&gt;</v>
+      </c>
+      <c r="L16" s="6" t="str">
+        <f t="shared" si="13"/>
+        <v>&lt;Button android:id="@+id/button62" android:layout_width="wrap_content" android:layout_height="wrap_content" android:minWidth="40dp" android:onClick="button62" app:layout_constraintEnd_toStartOf="@id/button63" app:layout_constraintHorizontal_weight="1" app:layout_constraintStart_toEndOf="@+id/button61" app:layout_constraintTop_toBottomOf="@id/button52" /&gt;</v>
+      </c>
+      <c r="M16" s="6" t="str">
+        <f t="shared" si="13"/>
+        <v>&lt;Button android:id="@+id/button63" android:layout_width="wrap_content" android:layout_height="wrap_content" android:minWidth="40dp" android:onClick="button63" app:layout_constraintEnd_toStartOf="@id/button64" app:layout_constraintHorizontal_weight="1" app:layout_constraintStart_toEndOf="@+id/button62" app:layout_constraintTop_toBottomOf="@id/button53" /&gt;</v>
+      </c>
+      <c r="N16" s="6" t="str">
+        <f t="shared" si="13"/>
+        <v>&lt;Button android:id="@+id/button64" android:layout_width="wrap_content" android:layout_height="wrap_content" android:minWidth="40dp" android:onClick="button64" app:layout_constraintEnd_toStartOf="@id/button65" app:layout_constraintHorizontal_weight="1" app:layout_constraintStart_toEndOf="@+id/button63" app:layout_constraintTop_toBottomOf="@id/button54" /&gt;</v>
+      </c>
+      <c r="O16" s="6" t="str">
+        <f t="shared" si="13"/>
+        <v>&lt;Button android:id="@+id/button65" android:layout_width="wrap_content" android:layout_height="wrap_content" android:minWidth="40dp" android:onClick="button65" app:layout_constraintEnd_toStartOf="@id/button66" app:layout_constraintHorizontal_weight="1" app:layout_constraintStart_toEndOf="@+id/button64" app:layout_constraintTop_toBottomOf="@id/button55" /&gt;</v>
+      </c>
+      <c r="P16" s="6" t="str">
+        <f t="shared" si="13"/>
+        <v>&lt;Button android:id="@+id/button66" android:layout_width="wrap_content" android:layout_height="wrap_content" android:minWidth="40dp" android:onClick="button66" app:layout_constraintEnd_toStartOf="@id/button67" app:layout_constraintHorizontal_weight="1" app:layout_constraintStart_toEndOf="@+id/button65" app:layout_constraintTop_toBottomOf="@id/button56" /&gt;</v>
+      </c>
+      <c r="Q16" s="6" t="str">
+        <f t="shared" si="13"/>
+        <v>&lt;Button android:id="@+id/button67" android:layout_width="wrap_content" android:layout_height="wrap_content" android:minWidth="40dp" android:onClick="button67" app:layout_constraintEnd_toStartOf="@id/button68" app:layout_constraintHorizontal_weight="1" app:layout_constraintStart_toEndOf="@+id/button66" app:layout_constraintTop_toBottomOf="@id/button57" /&gt;</v>
+      </c>
+      <c r="R16" s="6" t="str">
+        <f t="shared" si="13"/>
+        <v>&lt;Button android:id="@+id/button68" android:layout_width="wrap_content" android:layout_height="wrap_content" android:minWidth="40dp" android:onClick="button68" app:layout_constraintEnd_toStartOf="@id/button69" app:layout_constraintHorizontal_weight="1" app:layout_constraintStart_toEndOf="@+id/button67" app:layout_constraintTop_toBottomOf="@id/button58" /&gt;</v>
+      </c>
+      <c r="S16" s="8" t="str">
         <f t="shared" si="14"/>
-        <v>&lt;Button android:id="@+id/button69" android:layout_width="wrap_content" android:layout_height="wrap_content" android:layout_marginEnd="8dp" android:layout_marginRight="8dp" android:minWidth="40dp" android:text="O" app:layout_constraintEnd_toEndOf="parent" app:layout_constraintHorizontal_weight="1" app:layout_constraintStart_toEndOf="@id/button68" app:layout_constraintTop_toBottomOf="@id/button59" /&gt;</v>
+        <v>&lt;Button android:id="@+id/button69" android:layout_width="wrap_content" android:layout_height="wrap_content" android:layout_marginEnd="8dp" android:layout_marginRight="8dp" android:minWidth="40dp" android:onClick="button69" app:layout_constraintEnd_toEndOf="parent" app:layout_constraintHorizontal_weight="1" app:layout_constraintStart_toEndOf="@id/button68" app:layout_constraintTop_toBottomOf="@id/button59" /&gt;</v>
       </c>
     </row>
     <row r="17" spans="11:19" x14ac:dyDescent="0.25">
       <c r="K17" s="4" t="str">
         <f t="shared" si="12"/>
-        <v>&lt;Button android:id="@+id/button71" android:layout_width="wrap_content" android:layout_height="wrap_content" android:layout_marginLeft="8dp" android:layout_marginStart="8dp" android:minWidth="40dp" android:text="O" app:layout_constraintEnd_toStartOf="@id/button72" app:layout_constraintHorizontal_weight="1" app:layout_constraintStart_toStartOf="parent" app:layout_constraintTop_toBottomOf="@id/button61" /&gt;</v>
-      </c>
-      <c r="L17" t="str">
-        <f t="shared" ref="L17:R17" si="18">"&lt;Button android:id="&amp;CHAR(34)&amp;"@+id/"&amp;L7&amp;CHAR(34)&amp;" android:layout_width="&amp;CHAR(34)&amp;"wrap_content"&amp;CHAR(34)&amp;" android:layout_height="&amp;CHAR(34)&amp;"wrap_content"&amp;CHAR(34)&amp;" android:minWidth="&amp;CHAR(34)&amp;"40dp"&amp;CHAR(34)&amp;" android:text="&amp;CHAR(34)&amp;"O"&amp;CHAR(34)&amp;" app:layout_constraintEnd_toStartOf="&amp;CHAR(34)&amp;"@id/"&amp;M7&amp;CHAR(34)&amp;" app:layout_constraintHorizontal_weight="&amp;CHAR(34)&amp;"1"&amp;CHAR(34)&amp;" app:layout_constraintStart_toEndOf="&amp;CHAR(34)&amp;"@+id/"&amp;K7&amp;CHAR(34)&amp;" app:layout_constraintTop_toBottomOf="&amp;CHAR(34)&amp;"@id/"&amp;L6&amp;CHAR(34)&amp;" /&gt;"</f>
-        <v>&lt;Button android:id="@+id/button72" android:layout_width="wrap_content" android:layout_height="wrap_content" android:minWidth="40dp" android:text="O" app:layout_constraintEnd_toStartOf="@id/button73" app:layout_constraintHorizontal_weight="1" app:layout_constraintStart_toEndOf="@+id/button71" app:layout_constraintTop_toBottomOf="@id/button62" /&gt;</v>
-      </c>
-      <c r="M17" t="str">
-        <f t="shared" si="18"/>
-        <v>&lt;Button android:id="@+id/button73" android:layout_width="wrap_content" android:layout_height="wrap_content" android:minWidth="40dp" android:text="O" app:layout_constraintEnd_toStartOf="@id/button74" app:layout_constraintHorizontal_weight="1" app:layout_constraintStart_toEndOf="@+id/button72" app:layout_constraintTop_toBottomOf="@id/button63" /&gt;</v>
-      </c>
-      <c r="N17" t="str">
-        <f t="shared" si="18"/>
-        <v>&lt;Button android:id="@+id/button74" android:layout_width="wrap_content" android:layout_height="wrap_content" android:minWidth="40dp" android:text="O" app:layout_constraintEnd_toStartOf="@id/button75" app:layout_constraintHorizontal_weight="1" app:layout_constraintStart_toEndOf="@+id/button73" app:layout_constraintTop_toBottomOf="@id/button64" /&gt;</v>
-      </c>
-      <c r="O17" t="str">
-        <f t="shared" si="18"/>
-        <v>&lt;Button android:id="@+id/button75" android:layout_width="wrap_content" android:layout_height="wrap_content" android:minWidth="40dp" android:text="O" app:layout_constraintEnd_toStartOf="@id/button76" app:layout_constraintHorizontal_weight="1" app:layout_constraintStart_toEndOf="@+id/button74" app:layout_constraintTop_toBottomOf="@id/button65" /&gt;</v>
-      </c>
-      <c r="P17" t="str">
-        <f t="shared" si="18"/>
-        <v>&lt;Button android:id="@+id/button76" android:layout_width="wrap_content" android:layout_height="wrap_content" android:minWidth="40dp" android:text="O" app:layout_constraintEnd_toStartOf="@id/button77" app:layout_constraintHorizontal_weight="1" app:layout_constraintStart_toEndOf="@+id/button75" app:layout_constraintTop_toBottomOf="@id/button66" /&gt;</v>
-      </c>
-      <c r="Q17" t="str">
-        <f t="shared" si="18"/>
-        <v>&lt;Button android:id="@+id/button77" android:layout_width="wrap_content" android:layout_height="wrap_content" android:minWidth="40dp" android:text="O" app:layout_constraintEnd_toStartOf="@id/button78" app:layout_constraintHorizontal_weight="1" app:layout_constraintStart_toEndOf="@+id/button76" app:layout_constraintTop_toBottomOf="@id/button67" /&gt;</v>
-      </c>
-      <c r="R17" t="str">
-        <f t="shared" si="18"/>
-        <v>&lt;Button android:id="@+id/button78" android:layout_width="wrap_content" android:layout_height="wrap_content" android:minWidth="40dp" android:text="O" app:layout_constraintEnd_toStartOf="@id/button79" app:layout_constraintHorizontal_weight="1" app:layout_constraintStart_toEndOf="@+id/button77" app:layout_constraintTop_toBottomOf="@id/button68" /&gt;</v>
-      </c>
-      <c r="S17" s="4" t="str">
+        <v>&lt;Button android:id="@+id/button71" android:layout_width="wrap_content" android:layout_height="wrap_content" android:layout_marginLeft="8dp" android:layout_marginStart="8dp" android:minWidth="40dp" android:onClick="button71" app:layout_constraintEnd_toStartOf="@id/button72" app:layout_constraintHorizontal_weight="1" app:layout_constraintStart_toStartOf="parent" app:layout_constraintTop_toBottomOf="@id/button61" /&gt;</v>
+      </c>
+      <c r="L17" s="6" t="str">
+        <f t="shared" si="13"/>
+        <v>&lt;Button android:id="@+id/button72" android:layout_width="wrap_content" android:layout_height="wrap_content" android:minWidth="40dp" android:onClick="button72" app:layout_constraintEnd_toStartOf="@id/button73" app:layout_constraintHorizontal_weight="1" app:layout_constraintStart_toEndOf="@+id/button71" app:layout_constraintTop_toBottomOf="@id/button62" /&gt;</v>
+      </c>
+      <c r="M17" s="6" t="str">
+        <f t="shared" si="13"/>
+        <v>&lt;Button android:id="@+id/button73" android:layout_width="wrap_content" android:layout_height="wrap_content" android:minWidth="40dp" android:onClick="button73" app:layout_constraintEnd_toStartOf="@id/button74" app:layout_constraintHorizontal_weight="1" app:layout_constraintStart_toEndOf="@+id/button72" app:layout_constraintTop_toBottomOf="@id/button63" /&gt;</v>
+      </c>
+      <c r="N17" s="6" t="str">
+        <f t="shared" si="13"/>
+        <v>&lt;Button android:id="@+id/button74" android:layout_width="wrap_content" android:layout_height="wrap_content" android:minWidth="40dp" android:onClick="button74" app:layout_constraintEnd_toStartOf="@id/button75" app:layout_constraintHorizontal_weight="1" app:layout_constraintStart_toEndOf="@+id/button73" app:layout_constraintTop_toBottomOf="@id/button64" /&gt;</v>
+      </c>
+      <c r="O17" s="6" t="str">
+        <f t="shared" si="13"/>
+        <v>&lt;Button android:id="@+id/button75" android:layout_width="wrap_content" android:layout_height="wrap_content" android:minWidth="40dp" android:onClick="button75" app:layout_constraintEnd_toStartOf="@id/button76" app:layout_constraintHorizontal_weight="1" app:layout_constraintStart_toEndOf="@+id/button74" app:layout_constraintTop_toBottomOf="@id/button65" /&gt;</v>
+      </c>
+      <c r="P17" s="6" t="str">
+        <f t="shared" si="13"/>
+        <v>&lt;Button android:id="@+id/button76" android:layout_width="wrap_content" android:layout_height="wrap_content" android:minWidth="40dp" android:onClick="button76" app:layout_constraintEnd_toStartOf="@id/button77" app:layout_constraintHorizontal_weight="1" app:layout_constraintStart_toEndOf="@+id/button75" app:layout_constraintTop_toBottomOf="@id/button66" /&gt;</v>
+      </c>
+      <c r="Q17" s="6" t="str">
+        <f t="shared" si="13"/>
+        <v>&lt;Button android:id="@+id/button77" android:layout_width="wrap_content" android:layout_height="wrap_content" android:minWidth="40dp" android:onClick="button77" app:layout_constraintEnd_toStartOf="@id/button78" app:layout_constraintHorizontal_weight="1" app:layout_constraintStart_toEndOf="@+id/button76" app:layout_constraintTop_toBottomOf="@id/button67" /&gt;</v>
+      </c>
+      <c r="R17" s="6" t="str">
+        <f t="shared" si="13"/>
+        <v>&lt;Button android:id="@+id/button78" android:layout_width="wrap_content" android:layout_height="wrap_content" android:minWidth="40dp" android:onClick="button78" app:layout_constraintEnd_toStartOf="@id/button79" app:layout_constraintHorizontal_weight="1" app:layout_constraintStart_toEndOf="@+id/button77" app:layout_constraintTop_toBottomOf="@id/button68" /&gt;</v>
+      </c>
+      <c r="S17" s="8" t="str">
         <f t="shared" si="14"/>
-        <v>&lt;Button android:id="@+id/button79" android:layout_width="wrap_content" android:layout_height="wrap_content" android:layout_marginEnd="8dp" android:layout_marginRight="8dp" android:minWidth="40dp" android:text="O" app:layout_constraintEnd_toEndOf="parent" app:layout_constraintHorizontal_weight="1" app:layout_constraintStart_toEndOf="@id/button78" app:layout_constraintTop_toBottomOf="@id/button69" /&gt;</v>
+        <v>&lt;Button android:id="@+id/button79" android:layout_width="wrap_content" android:layout_height="wrap_content" android:layout_marginEnd="8dp" android:layout_marginRight="8dp" android:minWidth="40dp" android:onClick="button79" app:layout_constraintEnd_toEndOf="parent" app:layout_constraintHorizontal_weight="1" app:layout_constraintStart_toEndOf="@id/button78" app:layout_constraintTop_toBottomOf="@id/button69" /&gt;</v>
       </c>
     </row>
     <row r="18" spans="11:19" x14ac:dyDescent="0.25">
       <c r="K18" s="4" t="str">
         <f t="shared" si="12"/>
-        <v>&lt;Button android:id="@+id/button81" android:layout_width="wrap_content" android:layout_height="wrap_content" android:layout_marginLeft="8dp" android:layout_marginStart="8dp" android:minWidth="40dp" android:text="O" app:layout_constraintEnd_toStartOf="@id/button82" app:layout_constraintHorizontal_weight="1" app:layout_constraintStart_toStartOf="parent" app:layout_constraintTop_toBottomOf="@id/button71" /&gt;</v>
-      </c>
-      <c r="L18" t="str">
-        <f t="shared" ref="L18:R18" si="19">"&lt;Button android:id="&amp;CHAR(34)&amp;"@+id/"&amp;L8&amp;CHAR(34)&amp;" android:layout_width="&amp;CHAR(34)&amp;"wrap_content"&amp;CHAR(34)&amp;" android:layout_height="&amp;CHAR(34)&amp;"wrap_content"&amp;CHAR(34)&amp;" android:minWidth="&amp;CHAR(34)&amp;"40dp"&amp;CHAR(34)&amp;" android:text="&amp;CHAR(34)&amp;"O"&amp;CHAR(34)&amp;" app:layout_constraintEnd_toStartOf="&amp;CHAR(34)&amp;"@id/"&amp;M8&amp;CHAR(34)&amp;" app:layout_constraintHorizontal_weight="&amp;CHAR(34)&amp;"1"&amp;CHAR(34)&amp;" app:layout_constraintStart_toEndOf="&amp;CHAR(34)&amp;"@+id/"&amp;K8&amp;CHAR(34)&amp;" app:layout_constraintTop_toBottomOf="&amp;CHAR(34)&amp;"@id/"&amp;L7&amp;CHAR(34)&amp;" /&gt;"</f>
-        <v>&lt;Button android:id="@+id/button82" android:layout_width="wrap_content" android:layout_height="wrap_content" android:minWidth="40dp" android:text="O" app:layout_constraintEnd_toStartOf="@id/button83" app:layout_constraintHorizontal_weight="1" app:layout_constraintStart_toEndOf="@+id/button81" app:layout_constraintTop_toBottomOf="@id/button72" /&gt;</v>
-      </c>
-      <c r="M18" t="str">
-        <f t="shared" si="19"/>
-        <v>&lt;Button android:id="@+id/button83" android:layout_width="wrap_content" android:layout_height="wrap_content" android:minWidth="40dp" android:text="O" app:layout_constraintEnd_toStartOf="@id/button84" app:layout_constraintHorizontal_weight="1" app:layout_constraintStart_toEndOf="@+id/button82" app:layout_constraintTop_toBottomOf="@id/button73" /&gt;</v>
-      </c>
-      <c r="N18" t="str">
-        <f t="shared" si="19"/>
-        <v>&lt;Button android:id="@+id/button84" android:layout_width="wrap_content" android:layout_height="wrap_content" android:minWidth="40dp" android:text="O" app:layout_constraintEnd_toStartOf="@id/button85" app:layout_constraintHorizontal_weight="1" app:layout_constraintStart_toEndOf="@+id/button83" app:layout_constraintTop_toBottomOf="@id/button74" /&gt;</v>
-      </c>
-      <c r="O18" t="str">
-        <f t="shared" si="19"/>
-        <v>&lt;Button android:id="@+id/button85" android:layout_width="wrap_content" android:layout_height="wrap_content" android:minWidth="40dp" android:text="O" app:layout_constraintEnd_toStartOf="@id/button86" app:layout_constraintHorizontal_weight="1" app:layout_constraintStart_toEndOf="@+id/button84" app:layout_constraintTop_toBottomOf="@id/button75" /&gt;</v>
-      </c>
-      <c r="P18" t="str">
-        <f t="shared" si="19"/>
-        <v>&lt;Button android:id="@+id/button86" android:layout_width="wrap_content" android:layout_height="wrap_content" android:minWidth="40dp" android:text="O" app:layout_constraintEnd_toStartOf="@id/button87" app:layout_constraintHorizontal_weight="1" app:layout_constraintStart_toEndOf="@+id/button85" app:layout_constraintTop_toBottomOf="@id/button76" /&gt;</v>
-      </c>
-      <c r="Q18" t="str">
-        <f t="shared" si="19"/>
-        <v>&lt;Button android:id="@+id/button87" android:layout_width="wrap_content" android:layout_height="wrap_content" android:minWidth="40dp" android:text="O" app:layout_constraintEnd_toStartOf="@id/button88" app:layout_constraintHorizontal_weight="1" app:layout_constraintStart_toEndOf="@+id/button86" app:layout_constraintTop_toBottomOf="@id/button77" /&gt;</v>
-      </c>
-      <c r="R18" t="str">
-        <f t="shared" si="19"/>
-        <v>&lt;Button android:id="@+id/button88" android:layout_width="wrap_content" android:layout_height="wrap_content" android:minWidth="40dp" android:text="O" app:layout_constraintEnd_toStartOf="@id/button89" app:layout_constraintHorizontal_weight="1" app:layout_constraintStart_toEndOf="@+id/button87" app:layout_constraintTop_toBottomOf="@id/button78" /&gt;</v>
-      </c>
-      <c r="S18" s="4" t="str">
+        <v>&lt;Button android:id="@+id/button81" android:layout_width="wrap_content" android:layout_height="wrap_content" android:layout_marginLeft="8dp" android:layout_marginStart="8dp" android:minWidth="40dp" android:onClick="button81" app:layout_constraintEnd_toStartOf="@id/button82" app:layout_constraintHorizontal_weight="1" app:layout_constraintStart_toStartOf="parent" app:layout_constraintTop_toBottomOf="@id/button71" /&gt;</v>
+      </c>
+      <c r="L18" s="6" t="str">
+        <f t="shared" si="13"/>
+        <v>&lt;Button android:id="@+id/button82" android:layout_width="wrap_content" android:layout_height="wrap_content" android:minWidth="40dp" android:onClick="button82" app:layout_constraintEnd_toStartOf="@id/button83" app:layout_constraintHorizontal_weight="1" app:layout_constraintStart_toEndOf="@+id/button81" app:layout_constraintTop_toBottomOf="@id/button72" /&gt;</v>
+      </c>
+      <c r="M18" s="6" t="str">
+        <f t="shared" si="13"/>
+        <v>&lt;Button android:id="@+id/button83" android:layout_width="wrap_content" android:layout_height="wrap_content" android:minWidth="40dp" android:onClick="button83" app:layout_constraintEnd_toStartOf="@id/button84" app:layout_constraintHorizontal_weight="1" app:layout_constraintStart_toEndOf="@+id/button82" app:layout_constraintTop_toBottomOf="@id/button73" /&gt;</v>
+      </c>
+      <c r="N18" s="6" t="str">
+        <f t="shared" si="13"/>
+        <v>&lt;Button android:id="@+id/button84" android:layout_width="wrap_content" android:layout_height="wrap_content" android:minWidth="40dp" android:onClick="button84" app:layout_constraintEnd_toStartOf="@id/button85" app:layout_constraintHorizontal_weight="1" app:layout_constraintStart_toEndOf="@+id/button83" app:layout_constraintTop_toBottomOf="@id/button74" /&gt;</v>
+      </c>
+      <c r="O18" s="6" t="str">
+        <f t="shared" si="13"/>
+        <v>&lt;Button android:id="@+id/button85" android:layout_width="wrap_content" android:layout_height="wrap_content" android:minWidth="40dp" android:onClick="button85" app:layout_constraintEnd_toStartOf="@id/button86" app:layout_constraintHorizontal_weight="1" app:layout_constraintStart_toEndOf="@+id/button84" app:layout_constraintTop_toBottomOf="@id/button75" /&gt;</v>
+      </c>
+      <c r="P18" s="6" t="str">
+        <f t="shared" si="13"/>
+        <v>&lt;Button android:id="@+id/button86" android:layout_width="wrap_content" android:layout_height="wrap_content" android:minWidth="40dp" android:onClick="button86" app:layout_constraintEnd_toStartOf="@id/button87" app:layout_constraintHorizontal_weight="1" app:layout_constraintStart_toEndOf="@+id/button85" app:layout_constraintTop_toBottomOf="@id/button76" /&gt;</v>
+      </c>
+      <c r="Q18" s="6" t="str">
+        <f t="shared" si="13"/>
+        <v>&lt;Button android:id="@+id/button87" android:layout_width="wrap_content" android:layout_height="wrap_content" android:minWidth="40dp" android:onClick="button87" app:layout_constraintEnd_toStartOf="@id/button88" app:layout_constraintHorizontal_weight="1" app:layout_constraintStart_toEndOf="@+id/button86" app:layout_constraintTop_toBottomOf="@id/button77" /&gt;</v>
+      </c>
+      <c r="R18" s="6" t="str">
+        <f t="shared" si="13"/>
+        <v>&lt;Button android:id="@+id/button88" android:layout_width="wrap_content" android:layout_height="wrap_content" android:minWidth="40dp" android:onClick="button88" app:layout_constraintEnd_toStartOf="@id/button89" app:layout_constraintHorizontal_weight="1" app:layout_constraintStart_toEndOf="@+id/button87" app:layout_constraintTop_toBottomOf="@id/button78" /&gt;</v>
+      </c>
+      <c r="S18" s="8" t="str">
         <f t="shared" si="14"/>
-        <v>&lt;Button android:id="@+id/button89" android:layout_width="wrap_content" android:layout_height="wrap_content" android:layout_marginEnd="8dp" android:layout_marginRight="8dp" android:minWidth="40dp" android:text="O" app:layout_constraintEnd_toEndOf="parent" app:layout_constraintHorizontal_weight="1" app:layout_constraintStart_toEndOf="@id/button88" app:layout_constraintTop_toBottomOf="@id/button79" /&gt;</v>
+        <v>&lt;Button android:id="@+id/button89" android:layout_width="wrap_content" android:layout_height="wrap_content" android:layout_marginEnd="8dp" android:layout_marginRight="8dp" android:minWidth="40dp" android:onClick="button89" app:layout_constraintEnd_toEndOf="parent" app:layout_constraintHorizontal_weight="1" app:layout_constraintStart_toEndOf="@id/button88" app:layout_constraintTop_toBottomOf="@id/button79" /&gt;</v>
       </c>
     </row>
     <row r="19" spans="11:19" x14ac:dyDescent="0.25">
       <c r="K19" s="4" t="str">
         <f t="shared" si="12"/>
-        <v>&lt;Button android:id="@+id/button91" android:layout_width="wrap_content" android:layout_height="wrap_content" android:layout_marginLeft="8dp" android:layout_marginStart="8dp" android:minWidth="40dp" android:text="O" app:layout_constraintEnd_toStartOf="@id/button92" app:layout_constraintHorizontal_weight="1" app:layout_constraintStart_toStartOf="parent" app:layout_constraintTop_toBottomOf="@id/button81" /&gt;</v>
-      </c>
-      <c r="L19" t="str">
-        <f t="shared" ref="L19:R19" si="20">"&lt;Button android:id="&amp;CHAR(34)&amp;"@+id/"&amp;L9&amp;CHAR(34)&amp;" android:layout_width="&amp;CHAR(34)&amp;"wrap_content"&amp;CHAR(34)&amp;" android:layout_height="&amp;CHAR(34)&amp;"wrap_content"&amp;CHAR(34)&amp;" android:minWidth="&amp;CHAR(34)&amp;"40dp"&amp;CHAR(34)&amp;" android:text="&amp;CHAR(34)&amp;"O"&amp;CHAR(34)&amp;" app:layout_constraintEnd_toStartOf="&amp;CHAR(34)&amp;"@id/"&amp;M9&amp;CHAR(34)&amp;" app:layout_constraintHorizontal_weight="&amp;CHAR(34)&amp;"1"&amp;CHAR(34)&amp;" app:layout_constraintStart_toEndOf="&amp;CHAR(34)&amp;"@+id/"&amp;K9&amp;CHAR(34)&amp;" app:layout_constraintTop_toBottomOf="&amp;CHAR(34)&amp;"@id/"&amp;L8&amp;CHAR(34)&amp;" /&gt;"</f>
-        <v>&lt;Button android:id="@+id/button92" android:layout_width="wrap_content" android:layout_height="wrap_content" android:minWidth="40dp" android:text="O" app:layout_constraintEnd_toStartOf="@id/button93" app:layout_constraintHorizontal_weight="1" app:layout_constraintStart_toEndOf="@+id/button91" app:layout_constraintTop_toBottomOf="@id/button82" /&gt;</v>
-      </c>
-      <c r="M19" t="str">
-        <f t="shared" si="20"/>
-        <v>&lt;Button android:id="@+id/button93" android:layout_width="wrap_content" android:layout_height="wrap_content" android:minWidth="40dp" android:text="O" app:layout_constraintEnd_toStartOf="@id/button94" app:layout_constraintHorizontal_weight="1" app:layout_constraintStart_toEndOf="@+id/button92" app:layout_constraintTop_toBottomOf="@id/button83" /&gt;</v>
-      </c>
-      <c r="N19" t="str">
-        <f t="shared" si="20"/>
-        <v>&lt;Button android:id="@+id/button94" android:layout_width="wrap_content" android:layout_height="wrap_content" android:minWidth="40dp" android:text="O" app:layout_constraintEnd_toStartOf="@id/button95" app:layout_constraintHorizontal_weight="1" app:layout_constraintStart_toEndOf="@+id/button93" app:layout_constraintTop_toBottomOf="@id/button84" /&gt;</v>
-      </c>
-      <c r="O19" t="str">
-        <f t="shared" si="20"/>
-        <v>&lt;Button android:id="@+id/button95" android:layout_width="wrap_content" android:layout_height="wrap_content" android:minWidth="40dp" android:text="O" app:layout_constraintEnd_toStartOf="@id/button96" app:layout_constraintHorizontal_weight="1" app:layout_constraintStart_toEndOf="@+id/button94" app:layout_constraintTop_toBottomOf="@id/button85" /&gt;</v>
-      </c>
-      <c r="P19" t="str">
-        <f t="shared" si="20"/>
-        <v>&lt;Button android:id="@+id/button96" android:layout_width="wrap_content" android:layout_height="wrap_content" android:minWidth="40dp" android:text="O" app:layout_constraintEnd_toStartOf="@id/button97" app:layout_constraintHorizontal_weight="1" app:layout_constraintStart_toEndOf="@+id/button95" app:layout_constraintTop_toBottomOf="@id/button86" /&gt;</v>
-      </c>
-      <c r="Q19" t="str">
-        <f t="shared" si="20"/>
-        <v>&lt;Button android:id="@+id/button97" android:layout_width="wrap_content" android:layout_height="wrap_content" android:minWidth="40dp" android:text="O" app:layout_constraintEnd_toStartOf="@id/button98" app:layout_constraintHorizontal_weight="1" app:layout_constraintStart_toEndOf="@+id/button96" app:layout_constraintTop_toBottomOf="@id/button87" /&gt;</v>
-      </c>
-      <c r="R19" t="str">
-        <f t="shared" si="20"/>
-        <v>&lt;Button android:id="@+id/button98" android:layout_width="wrap_content" android:layout_height="wrap_content" android:minWidth="40dp" android:text="O" app:layout_constraintEnd_toStartOf="@id/button99" app:layout_constraintHorizontal_weight="1" app:layout_constraintStart_toEndOf="@+id/button97" app:layout_constraintTop_toBottomOf="@id/button88" /&gt;</v>
-      </c>
-      <c r="S19" s="4" t="str">
+        <v>&lt;Button android:id="@+id/button91" android:layout_width="wrap_content" android:layout_height="wrap_content" android:layout_marginLeft="8dp" android:layout_marginStart="8dp" android:minWidth="40dp" android:onClick="button91" app:layout_constraintEnd_toStartOf="@id/button92" app:layout_constraintHorizontal_weight="1" app:layout_constraintStart_toStartOf="parent" app:layout_constraintTop_toBottomOf="@id/button81" /&gt;</v>
+      </c>
+      <c r="L19" s="6" t="str">
+        <f t="shared" si="13"/>
+        <v>&lt;Button android:id="@+id/button92" android:layout_width="wrap_content" android:layout_height="wrap_content" android:minWidth="40dp" android:onClick="button92" app:layout_constraintEnd_toStartOf="@id/button93" app:layout_constraintHorizontal_weight="1" app:layout_constraintStart_toEndOf="@+id/button91" app:layout_constraintTop_toBottomOf="@id/button82" /&gt;</v>
+      </c>
+      <c r="M19" s="6" t="str">
+        <f t="shared" si="13"/>
+        <v>&lt;Button android:id="@+id/button93" android:layout_width="wrap_content" android:layout_height="wrap_content" android:minWidth="40dp" android:onClick="button93" app:layout_constraintEnd_toStartOf="@id/button94" app:layout_constraintHorizontal_weight="1" app:layout_constraintStart_toEndOf="@+id/button92" app:layout_constraintTop_toBottomOf="@id/button83" /&gt;</v>
+      </c>
+      <c r="N19" s="6" t="str">
+        <f t="shared" si="13"/>
+        <v>&lt;Button android:id="@+id/button94" android:layout_width="wrap_content" android:layout_height="wrap_content" android:minWidth="40dp" android:onClick="button94" app:layout_constraintEnd_toStartOf="@id/button95" app:layout_constraintHorizontal_weight="1" app:layout_constraintStart_toEndOf="@+id/button93" app:layout_constraintTop_toBottomOf="@id/button84" /&gt;</v>
+      </c>
+      <c r="O19" s="6" t="str">
+        <f t="shared" si="13"/>
+        <v>&lt;Button android:id="@+id/button95" android:layout_width="wrap_content" android:layout_height="wrap_content" android:minWidth="40dp" android:onClick="button95" app:layout_constraintEnd_toStartOf="@id/button96" app:layout_constraintHorizontal_weight="1" app:layout_constraintStart_toEndOf="@+id/button94" app:layout_constraintTop_toBottomOf="@id/button85" /&gt;</v>
+      </c>
+      <c r="P19" s="6" t="str">
+        <f t="shared" si="13"/>
+        <v>&lt;Button android:id="@+id/button96" android:layout_width="wrap_content" android:layout_height="wrap_content" android:minWidth="40dp" android:onClick="button96" app:layout_constraintEnd_toStartOf="@id/button97" app:layout_constraintHorizontal_weight="1" app:layout_constraintStart_toEndOf="@+id/button95" app:layout_constraintTop_toBottomOf="@id/button86" /&gt;</v>
+      </c>
+      <c r="Q19" s="6" t="str">
+        <f t="shared" si="13"/>
+        <v>&lt;Button android:id="@+id/button97" android:layout_width="wrap_content" android:layout_height="wrap_content" android:minWidth="40dp" android:onClick="button97" app:layout_constraintEnd_toStartOf="@id/button98" app:layout_constraintHorizontal_weight="1" app:layout_constraintStart_toEndOf="@+id/button96" app:layout_constraintTop_toBottomOf="@id/button87" /&gt;</v>
+      </c>
+      <c r="R19" s="6" t="str">
+        <f t="shared" si="13"/>
+        <v>&lt;Button android:id="@+id/button98" android:layout_width="wrap_content" android:layout_height="wrap_content" android:minWidth="40dp" android:onClick="button98" app:layout_constraintEnd_toStartOf="@id/button99" app:layout_constraintHorizontal_weight="1" app:layout_constraintStart_toEndOf="@+id/button97" app:layout_constraintTop_toBottomOf="@id/button88" /&gt;</v>
+      </c>
+      <c r="S19" s="8" t="str">
         <f t="shared" si="14"/>
-        <v>&lt;Button android:id="@+id/button99" android:layout_width="wrap_content" android:layout_height="wrap_content" android:layout_marginEnd="8dp" android:layout_marginRight="8dp" android:minWidth="40dp" android:text="O" app:layout_constraintEnd_toEndOf="parent" app:layout_constraintHorizontal_weight="1" app:layout_constraintStart_toEndOf="@id/button98" app:layout_constraintTop_toBottomOf="@id/button89" /&gt;</v>
+        <v>&lt;Button android:id="@+id/button99" android:layout_width="wrap_content" android:layout_height="wrap_content" android:layout_marginEnd="8dp" android:layout_marginRight="8dp" android:minWidth="40dp" android:onClick="button99" app:layout_constraintEnd_toEndOf="parent" app:layout_constraintHorizontal_weight="1" app:layout_constraintStart_toEndOf="@id/button98" app:layout_constraintTop_toBottomOf="@id/button89" /&gt;</v>
       </c>
     </row>
   </sheetData>
@@ -1590,8 +1628,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C81"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView topLeftCell="A60" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:C81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2655,5 +2693,576 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I20"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12:I20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="9" width="3" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
+      <c r="H1" s="9"/>
+      <c r="I1" s="9"/>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>2</v>
+      </c>
+      <c r="E2">
+        <v>2</v>
+      </c>
+      <c r="F2">
+        <v>2</v>
+      </c>
+      <c r="G2">
+        <v>3</v>
+      </c>
+      <c r="H2">
+        <v>3</v>
+      </c>
+      <c r="I2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>2</v>
+      </c>
+      <c r="E3">
+        <v>2</v>
+      </c>
+      <c r="F3">
+        <v>2</v>
+      </c>
+      <c r="G3">
+        <v>3</v>
+      </c>
+      <c r="H3">
+        <v>3</v>
+      </c>
+      <c r="I3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4">
+        <v>2</v>
+      </c>
+      <c r="E4">
+        <v>2</v>
+      </c>
+      <c r="F4">
+        <v>2</v>
+      </c>
+      <c r="G4">
+        <v>3</v>
+      </c>
+      <c r="H4">
+        <v>3</v>
+      </c>
+      <c r="I4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>4</v>
+      </c>
+      <c r="C5">
+        <v>4</v>
+      </c>
+      <c r="D5">
+        <v>5</v>
+      </c>
+      <c r="E5">
+        <v>5</v>
+      </c>
+      <c r="F5">
+        <v>5</v>
+      </c>
+      <c r="G5">
+        <v>6</v>
+      </c>
+      <c r="H5">
+        <v>6</v>
+      </c>
+      <c r="I5">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6">
+        <v>4</v>
+      </c>
+      <c r="C6">
+        <v>4</v>
+      </c>
+      <c r="D6">
+        <v>5</v>
+      </c>
+      <c r="E6">
+        <v>5</v>
+      </c>
+      <c r="F6">
+        <v>5</v>
+      </c>
+      <c r="G6">
+        <v>6</v>
+      </c>
+      <c r="H6">
+        <v>6</v>
+      </c>
+      <c r="I6">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>4</v>
+      </c>
+      <c r="B7">
+        <v>4</v>
+      </c>
+      <c r="C7">
+        <v>4</v>
+      </c>
+      <c r="D7">
+        <v>5</v>
+      </c>
+      <c r="E7">
+        <v>5</v>
+      </c>
+      <c r="F7">
+        <v>5</v>
+      </c>
+      <c r="G7">
+        <v>6</v>
+      </c>
+      <c r="H7">
+        <v>6</v>
+      </c>
+      <c r="I7">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>7</v>
+      </c>
+      <c r="C8">
+        <v>7</v>
+      </c>
+      <c r="D8">
+        <v>8</v>
+      </c>
+      <c r="E8">
+        <v>8</v>
+      </c>
+      <c r="F8">
+        <v>8</v>
+      </c>
+      <c r="G8">
+        <v>9</v>
+      </c>
+      <c r="H8">
+        <v>9</v>
+      </c>
+      <c r="I8">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>7</v>
+      </c>
+      <c r="B9">
+        <v>7</v>
+      </c>
+      <c r="C9">
+        <v>7</v>
+      </c>
+      <c r="D9">
+        <v>8</v>
+      </c>
+      <c r="E9">
+        <v>8</v>
+      </c>
+      <c r="F9">
+        <v>8</v>
+      </c>
+      <c r="G9">
+        <v>9</v>
+      </c>
+      <c r="H9">
+        <v>9</v>
+      </c>
+      <c r="I9">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>7</v>
+      </c>
+      <c r="B10">
+        <v>7</v>
+      </c>
+      <c r="C10">
+        <v>7</v>
+      </c>
+      <c r="D10">
+        <v>8</v>
+      </c>
+      <c r="E10">
+        <v>8</v>
+      </c>
+      <c r="F10">
+        <v>8</v>
+      </c>
+      <c r="G10">
+        <v>9</v>
+      </c>
+      <c r="H10">
+        <v>9</v>
+      </c>
+      <c r="I10">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="B11" s="9"/>
+      <c r="C11" s="9"/>
+      <c r="D11" s="9"/>
+      <c r="E11" s="9"/>
+      <c r="F11" s="9"/>
+      <c r="G11" s="9"/>
+      <c r="H11" s="9"/>
+      <c r="I11" s="9"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12">
+        <v>12</v>
+      </c>
+      <c r="C12">
+        <v>13</v>
+      </c>
+      <c r="D12">
+        <v>14</v>
+      </c>
+      <c r="E12">
+        <v>15</v>
+      </c>
+      <c r="F12">
+        <v>16</v>
+      </c>
+      <c r="G12">
+        <v>17</v>
+      </c>
+      <c r="H12">
+        <v>18</v>
+      </c>
+      <c r="I12">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>21</v>
+      </c>
+      <c r="B13">
+        <v>22</v>
+      </c>
+      <c r="C13">
+        <v>23</v>
+      </c>
+      <c r="D13">
+        <v>24</v>
+      </c>
+      <c r="E13">
+        <v>25</v>
+      </c>
+      <c r="F13">
+        <v>26</v>
+      </c>
+      <c r="G13">
+        <v>27</v>
+      </c>
+      <c r="H13">
+        <v>28</v>
+      </c>
+      <c r="I13">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>31</v>
+      </c>
+      <c r="B14">
+        <v>32</v>
+      </c>
+      <c r="C14">
+        <v>33</v>
+      </c>
+      <c r="D14">
+        <v>34</v>
+      </c>
+      <c r="E14">
+        <v>35</v>
+      </c>
+      <c r="F14">
+        <v>36</v>
+      </c>
+      <c r="G14">
+        <v>37</v>
+      </c>
+      <c r="H14">
+        <v>38</v>
+      </c>
+      <c r="I14">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>41</v>
+      </c>
+      <c r="B15">
+        <v>42</v>
+      </c>
+      <c r="C15">
+        <v>43</v>
+      </c>
+      <c r="D15">
+        <v>44</v>
+      </c>
+      <c r="E15">
+        <v>45</v>
+      </c>
+      <c r="F15">
+        <v>46</v>
+      </c>
+      <c r="G15">
+        <v>47</v>
+      </c>
+      <c r="H15">
+        <v>48</v>
+      </c>
+      <c r="I15">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>51</v>
+      </c>
+      <c r="B16">
+        <v>52</v>
+      </c>
+      <c r="C16">
+        <v>53</v>
+      </c>
+      <c r="D16">
+        <v>54</v>
+      </c>
+      <c r="E16">
+        <v>55</v>
+      </c>
+      <c r="F16">
+        <v>56</v>
+      </c>
+      <c r="G16">
+        <v>57</v>
+      </c>
+      <c r="H16">
+        <v>58</v>
+      </c>
+      <c r="I16">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>61</v>
+      </c>
+      <c r="B17">
+        <v>62</v>
+      </c>
+      <c r="C17">
+        <v>63</v>
+      </c>
+      <c r="D17">
+        <v>64</v>
+      </c>
+      <c r="E17">
+        <v>65</v>
+      </c>
+      <c r="F17">
+        <v>66</v>
+      </c>
+      <c r="G17">
+        <v>67</v>
+      </c>
+      <c r="H17">
+        <v>68</v>
+      </c>
+      <c r="I17">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>71</v>
+      </c>
+      <c r="B18">
+        <v>72</v>
+      </c>
+      <c r="C18">
+        <v>73</v>
+      </c>
+      <c r="D18">
+        <v>74</v>
+      </c>
+      <c r="E18">
+        <v>75</v>
+      </c>
+      <c r="F18">
+        <v>76</v>
+      </c>
+      <c r="G18">
+        <v>77</v>
+      </c>
+      <c r="H18">
+        <v>78</v>
+      </c>
+      <c r="I18">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>81</v>
+      </c>
+      <c r="B19">
+        <v>82</v>
+      </c>
+      <c r="C19">
+        <v>83</v>
+      </c>
+      <c r="D19">
+        <v>84</v>
+      </c>
+      <c r="E19">
+        <v>85</v>
+      </c>
+      <c r="F19">
+        <v>86</v>
+      </c>
+      <c r="G19">
+        <v>87</v>
+      </c>
+      <c r="H19">
+        <v>88</v>
+      </c>
+      <c r="I19">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>91</v>
+      </c>
+      <c r="B20">
+        <v>92</v>
+      </c>
+      <c r="C20">
+        <v>93</v>
+      </c>
+      <c r="D20">
+        <v>94</v>
+      </c>
+      <c r="E20">
+        <v>95</v>
+      </c>
+      <c r="F20">
+        <v>96</v>
+      </c>
+      <c r="G20">
+        <v>97</v>
+      </c>
+      <c r="H20">
+        <v>98</v>
+      </c>
+      <c r="I20">
+        <v>99</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:I1"/>
+    <mergeCell ref="A11:I11"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>